<commit_message>
Ya se pueden apuntar a los torneos y pelear, actualizando los datos de los participantes
</commit_message>
<xml_diff>
--- a/documentacion/Rubrica_TAREA3_AD_2025.xlsx
+++ b/documentacion/Rubrica_TAREA3_AD_2025.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capsx\Documents\trabajo\curso 2024-2025\Acceso Datos\ut3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raullg\OneDrive\DAM2\4 - Acceso a Datos\Segundo Trimestre\3-Trimestre-Pokemon-ADT-master\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC840CE-62FC-437F-97CC-5CAC0E0D4CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1488F53-BB8B-4BE4-A98E-EECE2FFB58BE}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="TAREA2AD_2024" sheetId="1" r:id="rId1"/>
@@ -404,7 +403,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,6 +502,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -909,9 +920,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -969,44 +977,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1020,12 +1004,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1342,450 +1374,450 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F84145B-2310-4C8F-B182-3774382571C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:QML86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="85" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="81" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="68"/>
+      <c r="C6" s="74" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="68"/>
+      <c r="C7" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="42" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="68"/>
+      <c r="C8" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="42" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="43" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="42" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="60" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="55"/>
+      <c r="C11" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="70"/>
+      <c r="D11" s="61"/>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="55"/>
+      <c r="C12" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="62" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="72"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="63"/>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="58" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="27" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="65"/>
+      <c r="D15" s="64"/>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="27" t="s">
+      <c r="B16" s="55"/>
+      <c r="C16" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="65"/>
+      <c r="D16" s="64"/>
     </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="27" t="s">
+      <c r="B17" s="55"/>
+      <c r="C17" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="65"/>
+      <c r="D17" s="64"/>
     </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="27" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="65"/>
+      <c r="D18" s="64"/>
     </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="27" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="65"/>
+      <c r="D19" s="64"/>
     </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="27" t="s">
+      <c r="B20" s="55"/>
+      <c r="C20" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="65"/>
+      <c r="D20" s="64"/>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="41" t="s">
+      <c r="B21" s="56"/>
+      <c r="C21" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="73"/>
+      <c r="D21" s="65"/>
     </row>
-    <row r="22" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="39" t="s">
+    <row r="22" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="27" t="s">
+      <c r="B23" s="55"/>
+      <c r="C23" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="69" t="s">
+      <c r="D23" s="60" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="70"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="61"/>
     </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="60"/>
-      <c r="C25" s="41" t="s">
+      <c r="B25" s="56"/>
+      <c r="C25" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="42" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="27" t="s">
+      <c r="B27" s="71"/>
+      <c r="C27" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="64" t="s">
+      <c r="B28" s="71"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="66" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="65"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="64"/>
     </row>
-    <row r="30" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="C30" s="27" t="s">
+      <c r="B30" s="71"/>
+      <c r="C30" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="57"/>
+      <c r="D30" s="59"/>
     </row>
-    <row r="31" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="43" t="s">
+      <c r="B31" s="71"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="27" t="s">
+      <c r="B32" s="71"/>
+      <c r="C32" s="74" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="41" t="s">
+      <c r="B33" s="72"/>
+      <c r="C33" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="56" t="s">
+      <c r="D34" s="58" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="27" t="s">
+      <c r="B35" s="55"/>
+      <c r="C35" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="57"/>
+      <c r="D35" s="59"/>
     </row>
-    <row r="36" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="64" t="s">
+      <c r="B36" s="55"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="66" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="65"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="64"/>
     </row>
-    <row r="38" spans="1:4" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="27" t="s">
+      <c r="B38" s="55"/>
+      <c r="C38" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="57"/>
+      <c r="D38" s="59"/>
     </row>
-    <row r="39" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="27" t="s">
+      <c r="B39" s="55"/>
+      <c r="C39" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="64" t="s">
+      <c r="D39" s="66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="59"/>
-      <c r="C40" s="41" t="s">
+      <c r="B40" s="55"/>
+      <c r="C40" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="65"/>
+      <c r="D40" s="64"/>
     </row>
-    <row r="41" spans="1:4" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="43" t="s">
+      <c r="D41" s="42" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="62"/>
+      <c r="B42" s="68"/>
       <c r="C42" s="27" t="s">
         <v>21</v>
       </c>
@@ -1793,1062 +1825,1062 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="62"/>
+      <c r="B43" s="68"/>
       <c r="C43" s="27"/>
-      <c r="D43" s="64" t="s">
+      <c r="D43" s="66" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="63"/>
-      <c r="C44" s="45" t="s">
+      <c r="B44" s="69"/>
+      <c r="C44" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="57"/>
+      <c r="D44" s="59"/>
     </row>
-    <row r="45" spans="1:4" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="39" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="59"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="43" t="s">
+      <c r="D46" s="42" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="59"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="27"/>
       <c r="D47" s="23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" s="2" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="60"/>
-      <c r="C48" s="41" t="s">
+      <c r="B48" s="56"/>
+      <c r="C48" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="43" t="s">
+      <c r="D48" s="42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:11842" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11842" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="73" t="s">
         <v>21</v>
       </c>
       <c r="D49" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:11842" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11842" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="62"/>
-      <c r="C50" s="27" t="s">
+      <c r="B50" s="68"/>
+      <c r="C50" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D50" s="64" t="s">
+      <c r="D50" s="66" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:11842" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11842" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B51" s="62"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="57"/>
+      <c r="B51" s="68"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="59"/>
     </row>
-    <row r="52" spans="1:11842" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11842" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="62"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="64" t="s">
+      <c r="B52" s="68"/>
+      <c r="C52" s="74"/>
+      <c r="D52" s="66" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:11842" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11842" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="62"/>
-      <c r="C53" s="27" t="s">
+      <c r="B53" s="68"/>
+      <c r="C53" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="65"/>
+      <c r="D53" s="64"/>
     </row>
-    <row r="54" spans="1:11842" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11842" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="62"/>
-      <c r="C54" s="27" t="s">
+      <c r="B54" s="68"/>
+      <c r="C54" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="65"/>
+      <c r="D54" s="64"/>
     </row>
-    <row r="55" spans="1:11842" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11842" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B55" s="63"/>
-      <c r="C55" s="45" t="s">
+      <c r="B55" s="69"/>
+      <c r="C55" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="65"/>
+      <c r="D55" s="64"/>
     </row>
-    <row r="56" spans="1:11842" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11842" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="54" t="s">
+      <c r="B56" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="40"/>
-      <c r="D56" s="56" t="s">
+      <c r="C56" s="73"/>
+      <c r="D56" s="58" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:11842" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11842" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="35"/>
-      <c r="N57" s="35"/>
-      <c r="O57" s="35"/>
-      <c r="P57" s="35"/>
-      <c r="Q57" s="35"/>
-      <c r="R57" s="35"/>
-      <c r="S57" s="35"/>
-      <c r="T57" s="35"/>
-      <c r="U57" s="35"/>
-      <c r="V57" s="35"/>
-      <c r="W57" s="35"/>
-      <c r="X57" s="35"/>
-      <c r="Y57" s="35"/>
-      <c r="Z57" s="35"/>
-      <c r="AA57" s="35"/>
-      <c r="AB57" s="35"/>
-      <c r="AC57" s="35"/>
-      <c r="AD57" s="35"/>
-      <c r="AE57" s="35"/>
-      <c r="AF57" s="35"/>
-      <c r="AG57" s="35"/>
-      <c r="AH57" s="35"/>
-      <c r="AI57" s="35"/>
-      <c r="AJ57" s="35"/>
-      <c r="AK57" s="35"/>
-      <c r="AL57" s="35"/>
-      <c r="AM57" s="35"/>
-      <c r="AN57" s="35"/>
-      <c r="AO57" s="35"/>
-      <c r="AP57" s="35"/>
-      <c r="AQ57" s="35"/>
-      <c r="AR57" s="35"/>
-      <c r="AS57" s="35"/>
-      <c r="AT57" s="35"/>
-      <c r="AU57" s="35"/>
-      <c r="AV57" s="35"/>
-      <c r="AW57" s="35"/>
-      <c r="AX57" s="35"/>
-      <c r="AY57" s="35"/>
-      <c r="AZ57" s="35"/>
-      <c r="BA57" s="35"/>
-      <c r="BB57" s="35"/>
-      <c r="BC57" s="35"/>
-      <c r="BD57" s="35"/>
-      <c r="BE57" s="35"/>
-      <c r="BF57" s="35"/>
-      <c r="BG57" s="35"/>
-      <c r="BH57" s="35"/>
-      <c r="BI57" s="35"/>
-      <c r="BJ57" s="35"/>
-      <c r="BK57" s="35"/>
-      <c r="BL57" s="35"/>
-      <c r="BM57" s="35"/>
-      <c r="BN57" s="35"/>
-      <c r="BO57" s="35"/>
-      <c r="BP57" s="35"/>
-      <c r="BQ57" s="35"/>
-      <c r="BR57" s="35"/>
-      <c r="BS57" s="35"/>
-      <c r="BT57" s="35"/>
-      <c r="BU57" s="35"/>
-      <c r="BV57" s="35"/>
-      <c r="BW57" s="35"/>
-      <c r="BX57" s="35"/>
-      <c r="BY57" s="35"/>
-      <c r="BZ57" s="35"/>
-      <c r="CA57" s="35"/>
-      <c r="CB57" s="35"/>
-      <c r="CC57" s="35"/>
-      <c r="CD57" s="35"/>
-      <c r="CE57" s="35"/>
-      <c r="CF57" s="35"/>
-      <c r="CG57" s="35"/>
-      <c r="CH57" s="35"/>
-      <c r="CI57" s="35"/>
-      <c r="CJ57" s="35"/>
-      <c r="CK57" s="35"/>
-      <c r="CL57" s="35"/>
-      <c r="CM57" s="35"/>
-      <c r="CN57" s="35"/>
-      <c r="CO57" s="35"/>
-      <c r="CP57" s="35"/>
-      <c r="CQ57" s="35"/>
-      <c r="CR57" s="35"/>
-      <c r="CS57" s="35"/>
-      <c r="CT57" s="35"/>
-      <c r="CU57" s="35"/>
-      <c r="CV57" s="35"/>
-      <c r="CW57" s="35"/>
-      <c r="CX57" s="35"/>
-      <c r="CY57" s="35"/>
-      <c r="CZ57" s="35"/>
-      <c r="DA57" s="35"/>
-      <c r="DB57" s="35"/>
-      <c r="DC57" s="35"/>
-      <c r="DD57" s="35"/>
-      <c r="DE57" s="35"/>
-      <c r="DF57" s="35"/>
-      <c r="DG57" s="35"/>
-      <c r="DH57" s="35"/>
-      <c r="DI57" s="35"/>
-      <c r="DJ57" s="35"/>
-      <c r="DK57" s="35"/>
-      <c r="DL57" s="35"/>
-      <c r="DM57" s="35"/>
-      <c r="DN57" s="35"/>
-      <c r="DO57" s="35"/>
-      <c r="DP57" s="35"/>
-      <c r="DQ57" s="35"/>
-      <c r="DR57" s="35"/>
-      <c r="DS57" s="35"/>
-      <c r="DT57" s="35"/>
-      <c r="DU57" s="35"/>
-      <c r="DV57" s="35"/>
-      <c r="DW57" s="35"/>
-      <c r="DX57" s="35"/>
-      <c r="DY57" s="35"/>
-      <c r="DZ57" s="35"/>
-      <c r="EA57" s="35"/>
-      <c r="EB57" s="35"/>
-      <c r="EC57" s="35"/>
-      <c r="ED57" s="35"/>
-      <c r="EE57" s="35"/>
-      <c r="EF57" s="35"/>
-      <c r="EG57" s="35"/>
-      <c r="EH57" s="35"/>
-      <c r="EI57" s="35"/>
-      <c r="EJ57" s="35"/>
-      <c r="EK57" s="35"/>
-      <c r="EL57" s="35"/>
-      <c r="EM57" s="35"/>
-      <c r="EN57" s="35"/>
-      <c r="EO57" s="35"/>
-      <c r="EP57" s="35"/>
-      <c r="EQ57" s="35"/>
-      <c r="ER57" s="35"/>
-      <c r="ES57" s="35"/>
-      <c r="ET57" s="35"/>
-      <c r="EU57" s="35"/>
-      <c r="EV57" s="35"/>
-      <c r="EW57" s="35"/>
-      <c r="EX57" s="35"/>
-      <c r="EY57" s="35"/>
-      <c r="EZ57" s="35"/>
-      <c r="FA57" s="35"/>
-      <c r="FB57" s="35"/>
-      <c r="FC57" s="35"/>
-      <c r="FD57" s="35"/>
-      <c r="FE57" s="35"/>
-      <c r="FF57" s="35"/>
-      <c r="FG57" s="35"/>
-      <c r="FH57" s="35"/>
-      <c r="FI57" s="35"/>
-      <c r="FJ57" s="35"/>
-      <c r="FK57" s="35"/>
-      <c r="FL57" s="35"/>
-      <c r="FM57" s="35"/>
-      <c r="FN57" s="35"/>
-      <c r="FO57" s="35"/>
-      <c r="FP57" s="35"/>
-      <c r="FQ57" s="35"/>
-      <c r="FR57" s="35"/>
-      <c r="FS57" s="35"/>
-      <c r="FT57" s="35"/>
-      <c r="FU57" s="35"/>
-      <c r="FV57" s="35"/>
-      <c r="FW57" s="35"/>
-      <c r="FX57" s="35"/>
-      <c r="FY57" s="35"/>
-      <c r="FZ57" s="35"/>
-      <c r="GA57" s="35"/>
-      <c r="GB57" s="35"/>
-      <c r="GC57" s="35"/>
-      <c r="GD57" s="35"/>
-      <c r="GE57" s="35"/>
-      <c r="GF57" s="35"/>
-      <c r="GG57" s="35"/>
-      <c r="GH57" s="35"/>
-      <c r="GI57" s="35"/>
-      <c r="GJ57" s="35"/>
-      <c r="GK57" s="35"/>
-      <c r="GL57" s="35"/>
-      <c r="GM57" s="35"/>
-      <c r="GN57" s="35"/>
-      <c r="GO57" s="35"/>
-      <c r="GP57" s="35"/>
-      <c r="GQ57" s="35"/>
-      <c r="GR57" s="35"/>
-      <c r="GS57" s="35"/>
-      <c r="GT57" s="35"/>
-      <c r="GU57" s="35"/>
-      <c r="GV57" s="35"/>
-      <c r="GW57" s="35"/>
-      <c r="GX57" s="35"/>
-      <c r="GY57" s="35"/>
-      <c r="GZ57" s="35"/>
-      <c r="HA57" s="35"/>
-      <c r="HB57" s="35"/>
-      <c r="HC57" s="35"/>
-      <c r="HD57" s="35"/>
-      <c r="HE57" s="35"/>
-      <c r="HF57" s="35"/>
-      <c r="HG57" s="35"/>
-      <c r="HH57" s="35"/>
-      <c r="HI57" s="35"/>
-      <c r="HJ57" s="35"/>
-      <c r="HK57" s="35"/>
-      <c r="HL57" s="35"/>
-      <c r="HM57" s="35"/>
-      <c r="HN57" s="35"/>
-      <c r="HO57" s="35"/>
-      <c r="HP57" s="35"/>
-      <c r="HQ57" s="35"/>
-      <c r="HR57" s="35"/>
-      <c r="HS57" s="35"/>
-      <c r="HT57" s="35"/>
-      <c r="HU57" s="35"/>
-      <c r="HV57" s="35"/>
-      <c r="HW57" s="35"/>
-      <c r="HX57" s="35"/>
-      <c r="HY57" s="35"/>
-      <c r="HZ57" s="35"/>
-      <c r="IA57" s="35"/>
-      <c r="IB57" s="35"/>
-      <c r="IC57" s="35"/>
-      <c r="ID57" s="35"/>
-      <c r="IE57" s="35"/>
-      <c r="IF57" s="35"/>
-      <c r="IG57" s="35"/>
-      <c r="IH57" s="35"/>
-      <c r="II57" s="35"/>
-      <c r="IJ57" s="35"/>
-      <c r="IK57" s="35"/>
-      <c r="IL57" s="35"/>
-      <c r="IM57" s="35"/>
-      <c r="IN57" s="35"/>
-      <c r="IO57" s="35"/>
-      <c r="IP57" s="35"/>
-      <c r="IQ57" s="35"/>
-      <c r="IR57" s="35"/>
-      <c r="IS57" s="35"/>
-      <c r="IT57" s="35"/>
-      <c r="IU57" s="35"/>
-      <c r="IV57" s="35"/>
-      <c r="IW57" s="35"/>
-      <c r="IX57" s="35"/>
-      <c r="IY57" s="35"/>
-      <c r="IZ57" s="35"/>
-      <c r="JA57" s="35"/>
-      <c r="JB57" s="35"/>
-      <c r="JC57" s="35"/>
-      <c r="JD57" s="35"/>
-      <c r="JE57" s="35"/>
-      <c r="JF57" s="35"/>
-      <c r="JG57" s="35"/>
-      <c r="JH57" s="35"/>
-      <c r="JI57" s="35"/>
-      <c r="JJ57" s="35"/>
-      <c r="JK57" s="35"/>
-      <c r="JL57" s="35"/>
-      <c r="JM57" s="35"/>
-      <c r="JN57" s="35"/>
-      <c r="JO57" s="35"/>
-      <c r="JP57" s="35"/>
-      <c r="JQ57" s="35"/>
-      <c r="JR57" s="35"/>
-      <c r="JS57" s="35"/>
-      <c r="JT57" s="35"/>
-      <c r="JU57" s="35"/>
-      <c r="JV57" s="35"/>
-      <c r="JW57" s="35"/>
-      <c r="JX57" s="35"/>
-      <c r="JY57" s="35"/>
-      <c r="JZ57" s="35"/>
-      <c r="KA57" s="35"/>
-      <c r="KB57" s="35"/>
-      <c r="KC57" s="35"/>
-      <c r="KD57" s="35"/>
-      <c r="KE57" s="35"/>
-      <c r="KF57" s="35"/>
-      <c r="KG57" s="35"/>
-      <c r="KH57" s="35"/>
-      <c r="KI57" s="35"/>
-      <c r="KJ57" s="35"/>
-      <c r="KK57" s="35"/>
-      <c r="KL57" s="35"/>
-      <c r="KM57" s="35"/>
-      <c r="KN57" s="35"/>
-      <c r="KO57" s="35"/>
-      <c r="KP57" s="35"/>
-      <c r="KQ57" s="35"/>
-      <c r="KR57" s="35"/>
-      <c r="KS57" s="35"/>
-      <c r="KT57" s="35"/>
-      <c r="KU57" s="35"/>
-      <c r="KV57" s="35"/>
-      <c r="KW57" s="35"/>
-      <c r="KX57" s="35"/>
-      <c r="KY57" s="35"/>
-      <c r="KZ57" s="35"/>
-      <c r="LA57" s="35"/>
-      <c r="LB57" s="35"/>
-      <c r="LC57" s="35"/>
-      <c r="LD57" s="35"/>
-      <c r="LE57" s="35"/>
-      <c r="LF57" s="35"/>
-      <c r="LG57" s="35"/>
-      <c r="LH57" s="35"/>
-      <c r="LI57" s="35"/>
-      <c r="LJ57" s="35"/>
-      <c r="LK57" s="35"/>
-      <c r="LL57" s="35"/>
-      <c r="LM57" s="35"/>
-      <c r="LN57" s="35"/>
-      <c r="LO57" s="35"/>
-      <c r="LP57" s="35"/>
-      <c r="LQ57" s="35"/>
-      <c r="LR57" s="35"/>
-      <c r="LS57" s="35"/>
-      <c r="LT57" s="35"/>
-      <c r="LU57" s="35"/>
-      <c r="LV57" s="35"/>
-      <c r="LW57" s="35"/>
-      <c r="LX57" s="35"/>
-      <c r="LY57" s="35"/>
-      <c r="LZ57" s="35"/>
-      <c r="MA57" s="35"/>
-      <c r="MB57" s="35"/>
-      <c r="MC57" s="35"/>
-      <c r="MD57" s="35"/>
-      <c r="ME57" s="35"/>
-      <c r="MF57" s="35"/>
-      <c r="MG57" s="35"/>
-      <c r="MH57" s="35"/>
-      <c r="MI57" s="35"/>
-      <c r="MJ57" s="35"/>
-      <c r="MK57" s="35"/>
-      <c r="ML57" s="35"/>
-      <c r="MM57" s="35"/>
-      <c r="MN57" s="35"/>
-      <c r="MO57" s="35"/>
-      <c r="MP57" s="35"/>
-      <c r="MQ57" s="35"/>
-      <c r="MR57" s="35"/>
-      <c r="MS57" s="35"/>
-      <c r="MT57" s="35"/>
-      <c r="MU57" s="35"/>
-      <c r="MV57" s="35"/>
-      <c r="MW57" s="35"/>
-      <c r="MX57" s="35"/>
-      <c r="MY57" s="35"/>
-      <c r="MZ57" s="35"/>
-      <c r="NA57" s="35"/>
-      <c r="NB57" s="35"/>
-      <c r="NC57" s="35"/>
-      <c r="ND57" s="35"/>
-      <c r="NE57" s="35"/>
-      <c r="NF57" s="35"/>
-      <c r="NG57" s="35"/>
-      <c r="NH57" s="35"/>
-      <c r="NI57" s="35"/>
-      <c r="NJ57" s="35"/>
-      <c r="NK57" s="35"/>
-      <c r="NL57" s="35"/>
-      <c r="NM57" s="35"/>
-      <c r="NN57" s="35"/>
-      <c r="NO57" s="35"/>
-      <c r="NP57" s="35"/>
-      <c r="NQ57" s="35"/>
-      <c r="NR57" s="35"/>
-      <c r="NS57" s="35"/>
-      <c r="NT57" s="35"/>
-      <c r="NU57" s="35"/>
-      <c r="NV57" s="35"/>
-      <c r="NW57" s="35"/>
-      <c r="NX57" s="35"/>
-      <c r="NY57" s="35"/>
-      <c r="NZ57" s="35"/>
-      <c r="OA57" s="35"/>
-      <c r="OB57" s="35"/>
-      <c r="OC57" s="35"/>
-      <c r="OD57" s="35"/>
-      <c r="OE57" s="35"/>
-      <c r="OF57" s="35"/>
-      <c r="OG57" s="35"/>
-      <c r="OH57" s="35"/>
-      <c r="OI57" s="35"/>
-      <c r="OJ57" s="35"/>
-      <c r="OK57" s="35"/>
-      <c r="OL57" s="35"/>
-      <c r="OM57" s="35"/>
-      <c r="ON57" s="35"/>
-      <c r="OO57" s="35"/>
-      <c r="OP57" s="35"/>
-      <c r="OQ57" s="35"/>
-      <c r="OR57" s="35"/>
-      <c r="OS57" s="35"/>
-      <c r="OT57" s="35"/>
-      <c r="OU57" s="35"/>
-      <c r="OV57" s="35"/>
-      <c r="OW57" s="35"/>
-      <c r="OX57" s="35"/>
-      <c r="OY57" s="35"/>
-      <c r="OZ57" s="35"/>
-      <c r="PA57" s="35"/>
-      <c r="PB57" s="35"/>
-      <c r="PC57" s="35"/>
-      <c r="PD57" s="35"/>
-      <c r="PE57" s="35"/>
-      <c r="PF57" s="35"/>
-      <c r="PG57" s="35"/>
-      <c r="PH57" s="35"/>
-      <c r="PI57" s="35"/>
-      <c r="PJ57" s="35"/>
-      <c r="PK57" s="35"/>
-      <c r="PL57" s="35"/>
-      <c r="PM57" s="35"/>
-      <c r="PN57" s="35"/>
-      <c r="PO57" s="35"/>
-      <c r="PP57" s="35"/>
-      <c r="PQ57" s="35"/>
-      <c r="PR57" s="35"/>
-      <c r="PS57" s="35"/>
-      <c r="PT57" s="35"/>
-      <c r="PU57" s="35"/>
-      <c r="PV57" s="35"/>
-      <c r="PW57" s="35"/>
-      <c r="PX57" s="35"/>
-      <c r="PY57" s="35"/>
-      <c r="PZ57" s="35"/>
-      <c r="QA57" s="35"/>
-      <c r="QB57" s="35"/>
-      <c r="QC57" s="35"/>
-      <c r="QD57" s="35"/>
-      <c r="QE57" s="35"/>
-      <c r="QF57" s="35"/>
-      <c r="QG57" s="35"/>
-      <c r="QH57" s="35"/>
-      <c r="QI57" s="35"/>
-      <c r="QJ57" s="35"/>
-      <c r="QK57" s="35"/>
-      <c r="QL57" s="35"/>
-      <c r="QM57" s="35"/>
-      <c r="QN57" s="35"/>
-      <c r="QO57" s="35"/>
-      <c r="QP57" s="35"/>
-      <c r="QQ57" s="35"/>
-      <c r="QR57" s="35"/>
-      <c r="QS57" s="35"/>
-      <c r="QT57" s="35"/>
-      <c r="QU57" s="35"/>
-      <c r="QV57" s="35"/>
-      <c r="QW57" s="35"/>
-      <c r="QX57" s="35"/>
-      <c r="QY57" s="35"/>
-      <c r="QZ57" s="35"/>
-      <c r="RA57" s="35"/>
-      <c r="RB57" s="35"/>
-      <c r="RC57" s="35"/>
-      <c r="RD57" s="35"/>
-      <c r="RE57" s="35"/>
-      <c r="RF57" s="35"/>
-      <c r="RG57" s="35"/>
-      <c r="RH57" s="35"/>
-      <c r="RI57" s="35"/>
-      <c r="RJ57" s="35"/>
-      <c r="RK57" s="35"/>
-      <c r="RL57" s="35"/>
-      <c r="RM57" s="35"/>
-      <c r="RN57" s="35"/>
-      <c r="RO57" s="35"/>
-      <c r="RP57" s="35"/>
-      <c r="RQ57" s="35"/>
-      <c r="RR57" s="35"/>
-      <c r="RS57" s="35"/>
-      <c r="RT57" s="35"/>
-      <c r="RU57" s="35"/>
-      <c r="RV57" s="35"/>
-      <c r="RW57" s="35"/>
-      <c r="RX57" s="35"/>
-      <c r="RY57" s="35"/>
-      <c r="RZ57" s="35"/>
-      <c r="SA57" s="35"/>
-      <c r="SB57" s="35"/>
-      <c r="SC57" s="35"/>
-      <c r="SD57" s="35"/>
-      <c r="SE57" s="35"/>
-      <c r="SF57" s="35"/>
-      <c r="SG57" s="35"/>
-      <c r="SH57" s="35"/>
-      <c r="SI57" s="35"/>
-      <c r="SJ57" s="35"/>
-      <c r="SK57" s="35"/>
-      <c r="SL57" s="35"/>
-      <c r="SM57" s="35"/>
-      <c r="SN57" s="35"/>
-      <c r="SO57" s="35"/>
-      <c r="SP57" s="35"/>
-      <c r="SQ57" s="35"/>
-      <c r="SR57" s="35"/>
-      <c r="SS57" s="35"/>
-      <c r="ST57" s="35"/>
-      <c r="SU57" s="35"/>
-      <c r="SV57" s="35"/>
-      <c r="SW57" s="35"/>
-      <c r="SX57" s="35"/>
-      <c r="SY57" s="35"/>
-      <c r="SZ57" s="35"/>
-      <c r="TA57" s="35"/>
-      <c r="TB57" s="35"/>
-      <c r="TC57" s="35"/>
-      <c r="TD57" s="35"/>
-      <c r="TE57" s="35"/>
-      <c r="TF57" s="35"/>
-      <c r="TG57" s="35"/>
-      <c r="TH57" s="35"/>
-      <c r="TI57" s="35"/>
-      <c r="TJ57" s="35"/>
-      <c r="TK57" s="35"/>
-      <c r="TL57" s="35"/>
-      <c r="TM57" s="35"/>
-      <c r="TN57" s="35"/>
-      <c r="TO57" s="35"/>
-      <c r="TP57" s="35"/>
-      <c r="TQ57" s="35"/>
-      <c r="TR57" s="35"/>
-      <c r="TS57" s="35"/>
-      <c r="TT57" s="35"/>
-      <c r="TU57" s="35"/>
-      <c r="TV57" s="35"/>
-      <c r="TW57" s="35"/>
-      <c r="TX57" s="35"/>
-      <c r="TY57" s="35"/>
-      <c r="TZ57" s="35"/>
-      <c r="UA57" s="35"/>
-      <c r="UB57" s="35"/>
-      <c r="UC57" s="35"/>
-      <c r="UD57" s="35"/>
-      <c r="UE57" s="35"/>
-      <c r="UF57" s="35"/>
-      <c r="UG57" s="35"/>
-      <c r="UH57" s="35"/>
-      <c r="UI57" s="35"/>
-      <c r="UJ57" s="35"/>
-      <c r="UK57" s="35"/>
-      <c r="UL57" s="35"/>
-      <c r="UM57" s="35"/>
-      <c r="UN57" s="35"/>
-      <c r="UO57" s="35"/>
-      <c r="UP57" s="35"/>
-      <c r="UQ57" s="35"/>
-      <c r="UR57" s="35"/>
-      <c r="US57" s="35"/>
-      <c r="UT57" s="35"/>
-      <c r="UU57" s="35"/>
-      <c r="UV57" s="35"/>
-      <c r="UW57" s="35"/>
-      <c r="UX57" s="35"/>
-      <c r="UY57" s="35"/>
-      <c r="UZ57" s="35"/>
-      <c r="VA57" s="35"/>
-      <c r="VB57" s="35"/>
-      <c r="VC57" s="35"/>
-      <c r="VD57" s="35"/>
-      <c r="VE57" s="35"/>
-      <c r="VF57" s="35"/>
-      <c r="VG57" s="35"/>
-      <c r="VH57" s="35"/>
-      <c r="VI57" s="35"/>
-      <c r="VJ57" s="35"/>
-      <c r="VK57" s="35"/>
-      <c r="VL57" s="35"/>
-      <c r="VM57" s="35"/>
-      <c r="VN57" s="35"/>
-      <c r="VO57" s="35"/>
-      <c r="VP57" s="35"/>
-      <c r="VQ57" s="35"/>
-      <c r="VR57" s="35"/>
-      <c r="VS57" s="35"/>
-      <c r="VT57" s="35"/>
-      <c r="VU57" s="35"/>
-      <c r="VV57" s="35"/>
-      <c r="VW57" s="35"/>
-      <c r="VX57" s="35"/>
-      <c r="VY57" s="35"/>
-      <c r="VZ57" s="35"/>
-      <c r="WA57" s="35"/>
-      <c r="WB57" s="35"/>
-      <c r="WC57" s="35"/>
-      <c r="WD57" s="35"/>
-      <c r="WE57" s="35"/>
-      <c r="WF57" s="35"/>
-      <c r="WG57" s="35"/>
-      <c r="WH57" s="35"/>
-      <c r="WI57" s="35"/>
-      <c r="WJ57" s="35"/>
-      <c r="WK57" s="35"/>
-      <c r="WL57" s="35"/>
-      <c r="WM57" s="35"/>
-      <c r="WN57" s="35"/>
-      <c r="WO57" s="35"/>
-      <c r="WP57" s="35"/>
-      <c r="WQ57" s="35"/>
-      <c r="WR57" s="35"/>
-      <c r="WS57" s="35"/>
-      <c r="WT57" s="35"/>
-      <c r="WU57" s="35"/>
-      <c r="WV57" s="35"/>
-      <c r="WW57" s="35"/>
-      <c r="WX57" s="35"/>
-      <c r="WY57" s="35"/>
-      <c r="WZ57" s="35"/>
-      <c r="XA57" s="35"/>
-      <c r="XB57" s="35"/>
-      <c r="XC57" s="35"/>
-      <c r="XD57" s="35"/>
-      <c r="XE57" s="35"/>
-      <c r="XF57" s="35"/>
-      <c r="XG57" s="35"/>
-      <c r="XH57" s="35"/>
-      <c r="XI57" s="35"/>
-      <c r="XJ57" s="35"/>
-      <c r="XK57" s="35"/>
-      <c r="XL57" s="35"/>
-      <c r="XM57" s="35"/>
-      <c r="XN57" s="35"/>
-      <c r="XO57" s="35"/>
-      <c r="XP57" s="35"/>
-      <c r="XQ57" s="35"/>
-      <c r="XR57" s="35"/>
-      <c r="XS57" s="35"/>
-      <c r="XT57" s="35"/>
-      <c r="XU57" s="35"/>
-      <c r="XV57" s="35"/>
-      <c r="XW57" s="35"/>
-      <c r="XX57" s="35"/>
-      <c r="XY57" s="35"/>
-      <c r="XZ57" s="35"/>
-      <c r="YA57" s="35"/>
-      <c r="YB57" s="35"/>
-      <c r="YC57" s="35"/>
-      <c r="YD57" s="35"/>
-      <c r="YE57" s="35"/>
-      <c r="YF57" s="35"/>
-      <c r="YG57" s="35"/>
-      <c r="YH57" s="35"/>
-      <c r="YI57" s="35"/>
-      <c r="YJ57" s="35"/>
-      <c r="YK57" s="35"/>
-      <c r="YL57" s="35"/>
-      <c r="YM57" s="35"/>
-      <c r="YN57" s="35"/>
-      <c r="YO57" s="35"/>
-      <c r="YP57" s="35"/>
-      <c r="YQ57" s="35"/>
-      <c r="YR57" s="35"/>
-      <c r="YS57" s="35"/>
-      <c r="YT57" s="35"/>
-      <c r="YU57" s="35"/>
-      <c r="YV57" s="35"/>
-      <c r="YW57" s="35"/>
-      <c r="YX57" s="35"/>
-      <c r="YY57" s="35"/>
-      <c r="YZ57" s="35"/>
-      <c r="ZA57" s="35"/>
-      <c r="ZB57" s="35"/>
-      <c r="ZC57" s="35"/>
-      <c r="ZD57" s="35"/>
-      <c r="ZE57" s="35"/>
-      <c r="ZF57" s="35"/>
-      <c r="ZG57" s="35"/>
-      <c r="ZH57" s="35"/>
-      <c r="ZI57" s="35"/>
-      <c r="ZJ57" s="35"/>
-      <c r="ZK57" s="35"/>
-      <c r="ZL57" s="35"/>
-      <c r="ZM57" s="35"/>
-      <c r="ZN57" s="35"/>
-      <c r="ZO57" s="35"/>
-      <c r="ZP57" s="35"/>
-      <c r="ZQ57" s="35"/>
-      <c r="ZR57" s="35"/>
-      <c r="ZS57" s="35"/>
-      <c r="ZT57" s="35"/>
-      <c r="ZU57" s="35"/>
-      <c r="ZV57" s="35"/>
-      <c r="ZW57" s="35"/>
-      <c r="ZX57" s="35"/>
-      <c r="ZY57" s="35"/>
-      <c r="ZZ57" s="35"/>
-      <c r="AAA57" s="35"/>
-      <c r="AAB57" s="35"/>
-      <c r="AAC57" s="35"/>
-      <c r="AAD57" s="35"/>
-      <c r="AAE57" s="35"/>
-      <c r="AAF57" s="35"/>
-      <c r="AAG57" s="35"/>
-      <c r="AAH57" s="35"/>
-      <c r="AAI57" s="35"/>
-      <c r="AAJ57" s="35"/>
-      <c r="AAK57" s="35"/>
-      <c r="AAL57" s="35"/>
-      <c r="AAM57" s="35"/>
-      <c r="AAN57" s="35"/>
-      <c r="AAO57" s="35"/>
-      <c r="AAP57" s="35"/>
-      <c r="AAQ57" s="35"/>
-      <c r="AAR57" s="35"/>
-      <c r="AAS57" s="35"/>
-      <c r="AAT57" s="35"/>
-      <c r="AAU57" s="35"/>
-      <c r="AAV57" s="35"/>
-      <c r="AAW57" s="35"/>
-      <c r="AAX57" s="35"/>
-      <c r="AAY57" s="35"/>
-      <c r="AAZ57" s="35"/>
-      <c r="ABA57" s="35"/>
-      <c r="ABB57" s="35"/>
-      <c r="ABC57" s="35"/>
-      <c r="ABD57" s="35"/>
-      <c r="ABE57" s="35"/>
-      <c r="ABF57" s="35"/>
-      <c r="ABG57" s="35"/>
-      <c r="ABH57" s="35"/>
-      <c r="ABI57" s="35"/>
-      <c r="ABJ57" s="35"/>
-      <c r="ABK57" s="35"/>
-      <c r="ABL57" s="35"/>
-      <c r="ABM57" s="35"/>
-      <c r="ABN57" s="35"/>
-      <c r="ABO57" s="35"/>
-      <c r="ABP57" s="35"/>
-      <c r="ABQ57" s="35"/>
-      <c r="ABR57" s="35"/>
-      <c r="ABS57" s="35"/>
-      <c r="ABT57" s="35"/>
-      <c r="ABU57" s="35"/>
-      <c r="ABV57" s="35"/>
-      <c r="ABW57" s="35"/>
-      <c r="ABX57" s="35"/>
-      <c r="ABY57" s="35"/>
-      <c r="ABZ57" s="35"/>
-      <c r="ACA57" s="35"/>
-      <c r="ACB57" s="35"/>
-      <c r="ACC57" s="35"/>
-      <c r="ACD57" s="35"/>
-      <c r="ACE57" s="35"/>
-      <c r="ACF57" s="35"/>
-      <c r="ACG57" s="35"/>
-      <c r="ACH57" s="35"/>
-      <c r="ACI57" s="35"/>
-      <c r="ACJ57" s="35"/>
-      <c r="ACK57" s="35"/>
-      <c r="ACL57" s="35"/>
-      <c r="ACM57" s="35"/>
-      <c r="ACN57" s="35"/>
-      <c r="ACO57" s="35"/>
-      <c r="ACP57" s="35"/>
-      <c r="ACQ57" s="35"/>
-      <c r="ACR57" s="35"/>
-      <c r="ACS57" s="35"/>
-      <c r="ACT57" s="35"/>
-      <c r="ACU57" s="35"/>
-      <c r="ACV57" s="35"/>
-      <c r="ACW57" s="35"/>
-      <c r="ACX57" s="35"/>
-      <c r="ACY57" s="35"/>
-      <c r="ACZ57" s="35"/>
-      <c r="ADA57" s="35"/>
-      <c r="ADB57" s="35"/>
-      <c r="ADC57" s="35"/>
-      <c r="ADD57" s="35"/>
-      <c r="ADE57" s="35"/>
-      <c r="ADF57" s="35"/>
-      <c r="ADG57" s="35"/>
-      <c r="ADH57" s="35"/>
-      <c r="ADI57" s="35"/>
-      <c r="ADJ57" s="35"/>
-      <c r="ADK57" s="35"/>
-      <c r="ADL57" s="35"/>
-      <c r="ADM57" s="35"/>
-      <c r="ADN57" s="35"/>
-      <c r="ADO57" s="35"/>
-      <c r="ADP57" s="35"/>
-      <c r="ADQ57" s="35"/>
-      <c r="ADR57" s="35"/>
-      <c r="ADS57" s="35"/>
-      <c r="ADT57" s="35"/>
-      <c r="ADU57" s="35"/>
-      <c r="ADV57" s="35"/>
-      <c r="ADW57" s="35"/>
-      <c r="ADX57" s="35"/>
-      <c r="ADY57" s="35"/>
-      <c r="ADZ57" s="35"/>
-      <c r="AEA57" s="35"/>
-      <c r="AEB57" s="35"/>
-      <c r="AEC57" s="35"/>
-      <c r="AED57" s="35"/>
-      <c r="AEE57" s="35"/>
-      <c r="AEF57" s="35"/>
-      <c r="AEG57" s="35"/>
-      <c r="AEH57" s="35"/>
-      <c r="AEI57" s="35"/>
-      <c r="AEJ57" s="35"/>
-      <c r="AEK57" s="35"/>
-      <c r="AEL57" s="35"/>
-      <c r="AEM57" s="35"/>
-      <c r="AEN57" s="35"/>
-      <c r="AEO57" s="35"/>
-      <c r="AEP57" s="35"/>
-      <c r="AEQ57" s="35"/>
-      <c r="AER57" s="35"/>
-      <c r="AES57" s="35"/>
-      <c r="AET57" s="35"/>
-      <c r="AEU57" s="35"/>
-      <c r="AEV57" s="35"/>
-      <c r="AEW57" s="35"/>
-      <c r="AEX57" s="35"/>
-      <c r="AEY57" s="35"/>
-      <c r="AEZ57" s="35"/>
-      <c r="AFA57" s="35"/>
-      <c r="AFB57" s="35"/>
-      <c r="AFC57" s="35"/>
-      <c r="AFD57" s="35"/>
-      <c r="AFE57" s="35"/>
-      <c r="AFF57" s="35"/>
-      <c r="AFG57" s="35"/>
-      <c r="AFH57" s="35"/>
-      <c r="AFI57" s="35"/>
-      <c r="AFJ57" s="35"/>
-      <c r="AFK57" s="35"/>
-      <c r="AFL57" s="35"/>
-      <c r="AFM57" s="35"/>
-      <c r="AFN57" s="35"/>
-      <c r="AFO57" s="35"/>
-      <c r="AFP57" s="35"/>
-      <c r="AFQ57" s="35"/>
-      <c r="AFR57" s="35"/>
-      <c r="AFS57" s="35"/>
-      <c r="AFT57" s="35"/>
-      <c r="AFU57" s="35"/>
-      <c r="AFV57" s="35"/>
-      <c r="AFW57" s="35"/>
-      <c r="AFX57" s="35"/>
-      <c r="AFY57" s="35"/>
-      <c r="AFZ57" s="35"/>
-      <c r="AGA57" s="35"/>
-      <c r="AGB57" s="35"/>
-      <c r="AGC57" s="35"/>
-      <c r="AGD57" s="35"/>
-      <c r="AGE57" s="35"/>
-      <c r="AGF57" s="35"/>
-      <c r="AGG57" s="35"/>
-      <c r="AGH57" s="35"/>
-      <c r="AGI57" s="35"/>
-      <c r="AGJ57" s="35"/>
-      <c r="AGK57" s="35"/>
-      <c r="AGL57" s="35"/>
-      <c r="AGM57" s="35"/>
-      <c r="AGN57" s="35"/>
-      <c r="AGO57" s="35"/>
-      <c r="AGP57" s="35"/>
-      <c r="AGQ57" s="35"/>
-      <c r="AGR57" s="35"/>
-      <c r="AGS57" s="35"/>
-      <c r="AGT57" s="35"/>
-      <c r="AGU57" s="35"/>
-      <c r="AGV57" s="35"/>
-      <c r="AGW57" s="35"/>
-      <c r="AGX57" s="35"/>
-      <c r="AGY57" s="35"/>
-      <c r="AGZ57" s="35"/>
-      <c r="AHA57" s="35"/>
-      <c r="AHB57" s="35"/>
-      <c r="AHC57" s="35"/>
-      <c r="AHD57" s="35"/>
-      <c r="AHE57" s="35"/>
-      <c r="AHF57" s="35"/>
-      <c r="AHG57" s="35"/>
-      <c r="AHH57" s="35"/>
-      <c r="AHI57" s="35"/>
-      <c r="AHJ57" s="35"/>
-      <c r="AHK57" s="35"/>
-      <c r="AHL57" s="35"/>
-      <c r="AHM57" s="35"/>
-      <c r="AHN57" s="35"/>
-      <c r="AHO57" s="35"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="77"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34"/>
+      <c r="N57" s="34"/>
+      <c r="O57" s="34"/>
+      <c r="P57" s="34"/>
+      <c r="Q57" s="34"/>
+      <c r="R57" s="34"/>
+      <c r="S57" s="34"/>
+      <c r="T57" s="34"/>
+      <c r="U57" s="34"/>
+      <c r="V57" s="34"/>
+      <c r="W57" s="34"/>
+      <c r="X57" s="34"/>
+      <c r="Y57" s="34"/>
+      <c r="Z57" s="34"/>
+      <c r="AA57" s="34"/>
+      <c r="AB57" s="34"/>
+      <c r="AC57" s="34"/>
+      <c r="AD57" s="34"/>
+      <c r="AE57" s="34"/>
+      <c r="AF57" s="34"/>
+      <c r="AG57" s="34"/>
+      <c r="AH57" s="34"/>
+      <c r="AI57" s="34"/>
+      <c r="AJ57" s="34"/>
+      <c r="AK57" s="34"/>
+      <c r="AL57" s="34"/>
+      <c r="AM57" s="34"/>
+      <c r="AN57" s="34"/>
+      <c r="AO57" s="34"/>
+      <c r="AP57" s="34"/>
+      <c r="AQ57" s="34"/>
+      <c r="AR57" s="34"/>
+      <c r="AS57" s="34"/>
+      <c r="AT57" s="34"/>
+      <c r="AU57" s="34"/>
+      <c r="AV57" s="34"/>
+      <c r="AW57" s="34"/>
+      <c r="AX57" s="34"/>
+      <c r="AY57" s="34"/>
+      <c r="AZ57" s="34"/>
+      <c r="BA57" s="34"/>
+      <c r="BB57" s="34"/>
+      <c r="BC57" s="34"/>
+      <c r="BD57" s="34"/>
+      <c r="BE57" s="34"/>
+      <c r="BF57" s="34"/>
+      <c r="BG57" s="34"/>
+      <c r="BH57" s="34"/>
+      <c r="BI57" s="34"/>
+      <c r="BJ57" s="34"/>
+      <c r="BK57" s="34"/>
+      <c r="BL57" s="34"/>
+      <c r="BM57" s="34"/>
+      <c r="BN57" s="34"/>
+      <c r="BO57" s="34"/>
+      <c r="BP57" s="34"/>
+      <c r="BQ57" s="34"/>
+      <c r="BR57" s="34"/>
+      <c r="BS57" s="34"/>
+      <c r="BT57" s="34"/>
+      <c r="BU57" s="34"/>
+      <c r="BV57" s="34"/>
+      <c r="BW57" s="34"/>
+      <c r="BX57" s="34"/>
+      <c r="BY57" s="34"/>
+      <c r="BZ57" s="34"/>
+      <c r="CA57" s="34"/>
+      <c r="CB57" s="34"/>
+      <c r="CC57" s="34"/>
+      <c r="CD57" s="34"/>
+      <c r="CE57" s="34"/>
+      <c r="CF57" s="34"/>
+      <c r="CG57" s="34"/>
+      <c r="CH57" s="34"/>
+      <c r="CI57" s="34"/>
+      <c r="CJ57" s="34"/>
+      <c r="CK57" s="34"/>
+      <c r="CL57" s="34"/>
+      <c r="CM57" s="34"/>
+      <c r="CN57" s="34"/>
+      <c r="CO57" s="34"/>
+      <c r="CP57" s="34"/>
+      <c r="CQ57" s="34"/>
+      <c r="CR57" s="34"/>
+      <c r="CS57" s="34"/>
+      <c r="CT57" s="34"/>
+      <c r="CU57" s="34"/>
+      <c r="CV57" s="34"/>
+      <c r="CW57" s="34"/>
+      <c r="CX57" s="34"/>
+      <c r="CY57" s="34"/>
+      <c r="CZ57" s="34"/>
+      <c r="DA57" s="34"/>
+      <c r="DB57" s="34"/>
+      <c r="DC57" s="34"/>
+      <c r="DD57" s="34"/>
+      <c r="DE57" s="34"/>
+      <c r="DF57" s="34"/>
+      <c r="DG57" s="34"/>
+      <c r="DH57" s="34"/>
+      <c r="DI57" s="34"/>
+      <c r="DJ57" s="34"/>
+      <c r="DK57" s="34"/>
+      <c r="DL57" s="34"/>
+      <c r="DM57" s="34"/>
+      <c r="DN57" s="34"/>
+      <c r="DO57" s="34"/>
+      <c r="DP57" s="34"/>
+      <c r="DQ57" s="34"/>
+      <c r="DR57" s="34"/>
+      <c r="DS57" s="34"/>
+      <c r="DT57" s="34"/>
+      <c r="DU57" s="34"/>
+      <c r="DV57" s="34"/>
+      <c r="DW57" s="34"/>
+      <c r="DX57" s="34"/>
+      <c r="DY57" s="34"/>
+      <c r="DZ57" s="34"/>
+      <c r="EA57" s="34"/>
+      <c r="EB57" s="34"/>
+      <c r="EC57" s="34"/>
+      <c r="ED57" s="34"/>
+      <c r="EE57" s="34"/>
+      <c r="EF57" s="34"/>
+      <c r="EG57" s="34"/>
+      <c r="EH57" s="34"/>
+      <c r="EI57" s="34"/>
+      <c r="EJ57" s="34"/>
+      <c r="EK57" s="34"/>
+      <c r="EL57" s="34"/>
+      <c r="EM57" s="34"/>
+      <c r="EN57" s="34"/>
+      <c r="EO57" s="34"/>
+      <c r="EP57" s="34"/>
+      <c r="EQ57" s="34"/>
+      <c r="ER57" s="34"/>
+      <c r="ES57" s="34"/>
+      <c r="ET57" s="34"/>
+      <c r="EU57" s="34"/>
+      <c r="EV57" s="34"/>
+      <c r="EW57" s="34"/>
+      <c r="EX57" s="34"/>
+      <c r="EY57" s="34"/>
+      <c r="EZ57" s="34"/>
+      <c r="FA57" s="34"/>
+      <c r="FB57" s="34"/>
+      <c r="FC57" s="34"/>
+      <c r="FD57" s="34"/>
+      <c r="FE57" s="34"/>
+      <c r="FF57" s="34"/>
+      <c r="FG57" s="34"/>
+      <c r="FH57" s="34"/>
+      <c r="FI57" s="34"/>
+      <c r="FJ57" s="34"/>
+      <c r="FK57" s="34"/>
+      <c r="FL57" s="34"/>
+      <c r="FM57" s="34"/>
+      <c r="FN57" s="34"/>
+      <c r="FO57" s="34"/>
+      <c r="FP57" s="34"/>
+      <c r="FQ57" s="34"/>
+      <c r="FR57" s="34"/>
+      <c r="FS57" s="34"/>
+      <c r="FT57" s="34"/>
+      <c r="FU57" s="34"/>
+      <c r="FV57" s="34"/>
+      <c r="FW57" s="34"/>
+      <c r="FX57" s="34"/>
+      <c r="FY57" s="34"/>
+      <c r="FZ57" s="34"/>
+      <c r="GA57" s="34"/>
+      <c r="GB57" s="34"/>
+      <c r="GC57" s="34"/>
+      <c r="GD57" s="34"/>
+      <c r="GE57" s="34"/>
+      <c r="GF57" s="34"/>
+      <c r="GG57" s="34"/>
+      <c r="GH57" s="34"/>
+      <c r="GI57" s="34"/>
+      <c r="GJ57" s="34"/>
+      <c r="GK57" s="34"/>
+      <c r="GL57" s="34"/>
+      <c r="GM57" s="34"/>
+      <c r="GN57" s="34"/>
+      <c r="GO57" s="34"/>
+      <c r="GP57" s="34"/>
+      <c r="GQ57" s="34"/>
+      <c r="GR57" s="34"/>
+      <c r="GS57" s="34"/>
+      <c r="GT57" s="34"/>
+      <c r="GU57" s="34"/>
+      <c r="GV57" s="34"/>
+      <c r="GW57" s="34"/>
+      <c r="GX57" s="34"/>
+      <c r="GY57" s="34"/>
+      <c r="GZ57" s="34"/>
+      <c r="HA57" s="34"/>
+      <c r="HB57" s="34"/>
+      <c r="HC57" s="34"/>
+      <c r="HD57" s="34"/>
+      <c r="HE57" s="34"/>
+      <c r="HF57" s="34"/>
+      <c r="HG57" s="34"/>
+      <c r="HH57" s="34"/>
+      <c r="HI57" s="34"/>
+      <c r="HJ57" s="34"/>
+      <c r="HK57" s="34"/>
+      <c r="HL57" s="34"/>
+      <c r="HM57" s="34"/>
+      <c r="HN57" s="34"/>
+      <c r="HO57" s="34"/>
+      <c r="HP57" s="34"/>
+      <c r="HQ57" s="34"/>
+      <c r="HR57" s="34"/>
+      <c r="HS57" s="34"/>
+      <c r="HT57" s="34"/>
+      <c r="HU57" s="34"/>
+      <c r="HV57" s="34"/>
+      <c r="HW57" s="34"/>
+      <c r="HX57" s="34"/>
+      <c r="HY57" s="34"/>
+      <c r="HZ57" s="34"/>
+      <c r="IA57" s="34"/>
+      <c r="IB57" s="34"/>
+      <c r="IC57" s="34"/>
+      <c r="ID57" s="34"/>
+      <c r="IE57" s="34"/>
+      <c r="IF57" s="34"/>
+      <c r="IG57" s="34"/>
+      <c r="IH57" s="34"/>
+      <c r="II57" s="34"/>
+      <c r="IJ57" s="34"/>
+      <c r="IK57" s="34"/>
+      <c r="IL57" s="34"/>
+      <c r="IM57" s="34"/>
+      <c r="IN57" s="34"/>
+      <c r="IO57" s="34"/>
+      <c r="IP57" s="34"/>
+      <c r="IQ57" s="34"/>
+      <c r="IR57" s="34"/>
+      <c r="IS57" s="34"/>
+      <c r="IT57" s="34"/>
+      <c r="IU57" s="34"/>
+      <c r="IV57" s="34"/>
+      <c r="IW57" s="34"/>
+      <c r="IX57" s="34"/>
+      <c r="IY57" s="34"/>
+      <c r="IZ57" s="34"/>
+      <c r="JA57" s="34"/>
+      <c r="JB57" s="34"/>
+      <c r="JC57" s="34"/>
+      <c r="JD57" s="34"/>
+      <c r="JE57" s="34"/>
+      <c r="JF57" s="34"/>
+      <c r="JG57" s="34"/>
+      <c r="JH57" s="34"/>
+      <c r="JI57" s="34"/>
+      <c r="JJ57" s="34"/>
+      <c r="JK57" s="34"/>
+      <c r="JL57" s="34"/>
+      <c r="JM57" s="34"/>
+      <c r="JN57" s="34"/>
+      <c r="JO57" s="34"/>
+      <c r="JP57" s="34"/>
+      <c r="JQ57" s="34"/>
+      <c r="JR57" s="34"/>
+      <c r="JS57" s="34"/>
+      <c r="JT57" s="34"/>
+      <c r="JU57" s="34"/>
+      <c r="JV57" s="34"/>
+      <c r="JW57" s="34"/>
+      <c r="JX57" s="34"/>
+      <c r="JY57" s="34"/>
+      <c r="JZ57" s="34"/>
+      <c r="KA57" s="34"/>
+      <c r="KB57" s="34"/>
+      <c r="KC57" s="34"/>
+      <c r="KD57" s="34"/>
+      <c r="KE57" s="34"/>
+      <c r="KF57" s="34"/>
+      <c r="KG57" s="34"/>
+      <c r="KH57" s="34"/>
+      <c r="KI57" s="34"/>
+      <c r="KJ57" s="34"/>
+      <c r="KK57" s="34"/>
+      <c r="KL57" s="34"/>
+      <c r="KM57" s="34"/>
+      <c r="KN57" s="34"/>
+      <c r="KO57" s="34"/>
+      <c r="KP57" s="34"/>
+      <c r="KQ57" s="34"/>
+      <c r="KR57" s="34"/>
+      <c r="KS57" s="34"/>
+      <c r="KT57" s="34"/>
+      <c r="KU57" s="34"/>
+      <c r="KV57" s="34"/>
+      <c r="KW57" s="34"/>
+      <c r="KX57" s="34"/>
+      <c r="KY57" s="34"/>
+      <c r="KZ57" s="34"/>
+      <c r="LA57" s="34"/>
+      <c r="LB57" s="34"/>
+      <c r="LC57" s="34"/>
+      <c r="LD57" s="34"/>
+      <c r="LE57" s="34"/>
+      <c r="LF57" s="34"/>
+      <c r="LG57" s="34"/>
+      <c r="LH57" s="34"/>
+      <c r="LI57" s="34"/>
+      <c r="LJ57" s="34"/>
+      <c r="LK57" s="34"/>
+      <c r="LL57" s="34"/>
+      <c r="LM57" s="34"/>
+      <c r="LN57" s="34"/>
+      <c r="LO57" s="34"/>
+      <c r="LP57" s="34"/>
+      <c r="LQ57" s="34"/>
+      <c r="LR57" s="34"/>
+      <c r="LS57" s="34"/>
+      <c r="LT57" s="34"/>
+      <c r="LU57" s="34"/>
+      <c r="LV57" s="34"/>
+      <c r="LW57" s="34"/>
+      <c r="LX57" s="34"/>
+      <c r="LY57" s="34"/>
+      <c r="LZ57" s="34"/>
+      <c r="MA57" s="34"/>
+      <c r="MB57" s="34"/>
+      <c r="MC57" s="34"/>
+      <c r="MD57" s="34"/>
+      <c r="ME57" s="34"/>
+      <c r="MF57" s="34"/>
+      <c r="MG57" s="34"/>
+      <c r="MH57" s="34"/>
+      <c r="MI57" s="34"/>
+      <c r="MJ57" s="34"/>
+      <c r="MK57" s="34"/>
+      <c r="ML57" s="34"/>
+      <c r="MM57" s="34"/>
+      <c r="MN57" s="34"/>
+      <c r="MO57" s="34"/>
+      <c r="MP57" s="34"/>
+      <c r="MQ57" s="34"/>
+      <c r="MR57" s="34"/>
+      <c r="MS57" s="34"/>
+      <c r="MT57" s="34"/>
+      <c r="MU57" s="34"/>
+      <c r="MV57" s="34"/>
+      <c r="MW57" s="34"/>
+      <c r="MX57" s="34"/>
+      <c r="MY57" s="34"/>
+      <c r="MZ57" s="34"/>
+      <c r="NA57" s="34"/>
+      <c r="NB57" s="34"/>
+      <c r="NC57" s="34"/>
+      <c r="ND57" s="34"/>
+      <c r="NE57" s="34"/>
+      <c r="NF57" s="34"/>
+      <c r="NG57" s="34"/>
+      <c r="NH57" s="34"/>
+      <c r="NI57" s="34"/>
+      <c r="NJ57" s="34"/>
+      <c r="NK57" s="34"/>
+      <c r="NL57" s="34"/>
+      <c r="NM57" s="34"/>
+      <c r="NN57" s="34"/>
+      <c r="NO57" s="34"/>
+      <c r="NP57" s="34"/>
+      <c r="NQ57" s="34"/>
+      <c r="NR57" s="34"/>
+      <c r="NS57" s="34"/>
+      <c r="NT57" s="34"/>
+      <c r="NU57" s="34"/>
+      <c r="NV57" s="34"/>
+      <c r="NW57" s="34"/>
+      <c r="NX57" s="34"/>
+      <c r="NY57" s="34"/>
+      <c r="NZ57" s="34"/>
+      <c r="OA57" s="34"/>
+      <c r="OB57" s="34"/>
+      <c r="OC57" s="34"/>
+      <c r="OD57" s="34"/>
+      <c r="OE57" s="34"/>
+      <c r="OF57" s="34"/>
+      <c r="OG57" s="34"/>
+      <c r="OH57" s="34"/>
+      <c r="OI57" s="34"/>
+      <c r="OJ57" s="34"/>
+      <c r="OK57" s="34"/>
+      <c r="OL57" s="34"/>
+      <c r="OM57" s="34"/>
+      <c r="ON57" s="34"/>
+      <c r="OO57" s="34"/>
+      <c r="OP57" s="34"/>
+      <c r="OQ57" s="34"/>
+      <c r="OR57" s="34"/>
+      <c r="OS57" s="34"/>
+      <c r="OT57" s="34"/>
+      <c r="OU57" s="34"/>
+      <c r="OV57" s="34"/>
+      <c r="OW57" s="34"/>
+      <c r="OX57" s="34"/>
+      <c r="OY57" s="34"/>
+      <c r="OZ57" s="34"/>
+      <c r="PA57" s="34"/>
+      <c r="PB57" s="34"/>
+      <c r="PC57" s="34"/>
+      <c r="PD57" s="34"/>
+      <c r="PE57" s="34"/>
+      <c r="PF57" s="34"/>
+      <c r="PG57" s="34"/>
+      <c r="PH57" s="34"/>
+      <c r="PI57" s="34"/>
+      <c r="PJ57" s="34"/>
+      <c r="PK57" s="34"/>
+      <c r="PL57" s="34"/>
+      <c r="PM57" s="34"/>
+      <c r="PN57" s="34"/>
+      <c r="PO57" s="34"/>
+      <c r="PP57" s="34"/>
+      <c r="PQ57" s="34"/>
+      <c r="PR57" s="34"/>
+      <c r="PS57" s="34"/>
+      <c r="PT57" s="34"/>
+      <c r="PU57" s="34"/>
+      <c r="PV57" s="34"/>
+      <c r="PW57" s="34"/>
+      <c r="PX57" s="34"/>
+      <c r="PY57" s="34"/>
+      <c r="PZ57" s="34"/>
+      <c r="QA57" s="34"/>
+      <c r="QB57" s="34"/>
+      <c r="QC57" s="34"/>
+      <c r="QD57" s="34"/>
+      <c r="QE57" s="34"/>
+      <c r="QF57" s="34"/>
+      <c r="QG57" s="34"/>
+      <c r="QH57" s="34"/>
+      <c r="QI57" s="34"/>
+      <c r="QJ57" s="34"/>
+      <c r="QK57" s="34"/>
+      <c r="QL57" s="34"/>
+      <c r="QM57" s="34"/>
+      <c r="QN57" s="34"/>
+      <c r="QO57" s="34"/>
+      <c r="QP57" s="34"/>
+      <c r="QQ57" s="34"/>
+      <c r="QR57" s="34"/>
+      <c r="QS57" s="34"/>
+      <c r="QT57" s="34"/>
+      <c r="QU57" s="34"/>
+      <c r="QV57" s="34"/>
+      <c r="QW57" s="34"/>
+      <c r="QX57" s="34"/>
+      <c r="QY57" s="34"/>
+      <c r="QZ57" s="34"/>
+      <c r="RA57" s="34"/>
+      <c r="RB57" s="34"/>
+      <c r="RC57" s="34"/>
+      <c r="RD57" s="34"/>
+      <c r="RE57" s="34"/>
+      <c r="RF57" s="34"/>
+      <c r="RG57" s="34"/>
+      <c r="RH57" s="34"/>
+      <c r="RI57" s="34"/>
+      <c r="RJ57" s="34"/>
+      <c r="RK57" s="34"/>
+      <c r="RL57" s="34"/>
+      <c r="RM57" s="34"/>
+      <c r="RN57" s="34"/>
+      <c r="RO57" s="34"/>
+      <c r="RP57" s="34"/>
+      <c r="RQ57" s="34"/>
+      <c r="RR57" s="34"/>
+      <c r="RS57" s="34"/>
+      <c r="RT57" s="34"/>
+      <c r="RU57" s="34"/>
+      <c r="RV57" s="34"/>
+      <c r="RW57" s="34"/>
+      <c r="RX57" s="34"/>
+      <c r="RY57" s="34"/>
+      <c r="RZ57" s="34"/>
+      <c r="SA57" s="34"/>
+      <c r="SB57" s="34"/>
+      <c r="SC57" s="34"/>
+      <c r="SD57" s="34"/>
+      <c r="SE57" s="34"/>
+      <c r="SF57" s="34"/>
+      <c r="SG57" s="34"/>
+      <c r="SH57" s="34"/>
+      <c r="SI57" s="34"/>
+      <c r="SJ57" s="34"/>
+      <c r="SK57" s="34"/>
+      <c r="SL57" s="34"/>
+      <c r="SM57" s="34"/>
+      <c r="SN57" s="34"/>
+      <c r="SO57" s="34"/>
+      <c r="SP57" s="34"/>
+      <c r="SQ57" s="34"/>
+      <c r="SR57" s="34"/>
+      <c r="SS57" s="34"/>
+      <c r="ST57" s="34"/>
+      <c r="SU57" s="34"/>
+      <c r="SV57" s="34"/>
+      <c r="SW57" s="34"/>
+      <c r="SX57" s="34"/>
+      <c r="SY57" s="34"/>
+      <c r="SZ57" s="34"/>
+      <c r="TA57" s="34"/>
+      <c r="TB57" s="34"/>
+      <c r="TC57" s="34"/>
+      <c r="TD57" s="34"/>
+      <c r="TE57" s="34"/>
+      <c r="TF57" s="34"/>
+      <c r="TG57" s="34"/>
+      <c r="TH57" s="34"/>
+      <c r="TI57" s="34"/>
+      <c r="TJ57" s="34"/>
+      <c r="TK57" s="34"/>
+      <c r="TL57" s="34"/>
+      <c r="TM57" s="34"/>
+      <c r="TN57" s="34"/>
+      <c r="TO57" s="34"/>
+      <c r="TP57" s="34"/>
+      <c r="TQ57" s="34"/>
+      <c r="TR57" s="34"/>
+      <c r="TS57" s="34"/>
+      <c r="TT57" s="34"/>
+      <c r="TU57" s="34"/>
+      <c r="TV57" s="34"/>
+      <c r="TW57" s="34"/>
+      <c r="TX57" s="34"/>
+      <c r="TY57" s="34"/>
+      <c r="TZ57" s="34"/>
+      <c r="UA57" s="34"/>
+      <c r="UB57" s="34"/>
+      <c r="UC57" s="34"/>
+      <c r="UD57" s="34"/>
+      <c r="UE57" s="34"/>
+      <c r="UF57" s="34"/>
+      <c r="UG57" s="34"/>
+      <c r="UH57" s="34"/>
+      <c r="UI57" s="34"/>
+      <c r="UJ57" s="34"/>
+      <c r="UK57" s="34"/>
+      <c r="UL57" s="34"/>
+      <c r="UM57" s="34"/>
+      <c r="UN57" s="34"/>
+      <c r="UO57" s="34"/>
+      <c r="UP57" s="34"/>
+      <c r="UQ57" s="34"/>
+      <c r="UR57" s="34"/>
+      <c r="US57" s="34"/>
+      <c r="UT57" s="34"/>
+      <c r="UU57" s="34"/>
+      <c r="UV57" s="34"/>
+      <c r="UW57" s="34"/>
+      <c r="UX57" s="34"/>
+      <c r="UY57" s="34"/>
+      <c r="UZ57" s="34"/>
+      <c r="VA57" s="34"/>
+      <c r="VB57" s="34"/>
+      <c r="VC57" s="34"/>
+      <c r="VD57" s="34"/>
+      <c r="VE57" s="34"/>
+      <c r="VF57" s="34"/>
+      <c r="VG57" s="34"/>
+      <c r="VH57" s="34"/>
+      <c r="VI57" s="34"/>
+      <c r="VJ57" s="34"/>
+      <c r="VK57" s="34"/>
+      <c r="VL57" s="34"/>
+      <c r="VM57" s="34"/>
+      <c r="VN57" s="34"/>
+      <c r="VO57" s="34"/>
+      <c r="VP57" s="34"/>
+      <c r="VQ57" s="34"/>
+      <c r="VR57" s="34"/>
+      <c r="VS57" s="34"/>
+      <c r="VT57" s="34"/>
+      <c r="VU57" s="34"/>
+      <c r="VV57" s="34"/>
+      <c r="VW57" s="34"/>
+      <c r="VX57" s="34"/>
+      <c r="VY57" s="34"/>
+      <c r="VZ57" s="34"/>
+      <c r="WA57" s="34"/>
+      <c r="WB57" s="34"/>
+      <c r="WC57" s="34"/>
+      <c r="WD57" s="34"/>
+      <c r="WE57" s="34"/>
+      <c r="WF57" s="34"/>
+      <c r="WG57" s="34"/>
+      <c r="WH57" s="34"/>
+      <c r="WI57" s="34"/>
+      <c r="WJ57" s="34"/>
+      <c r="WK57" s="34"/>
+      <c r="WL57" s="34"/>
+      <c r="WM57" s="34"/>
+      <c r="WN57" s="34"/>
+      <c r="WO57" s="34"/>
+      <c r="WP57" s="34"/>
+      <c r="WQ57" s="34"/>
+      <c r="WR57" s="34"/>
+      <c r="WS57" s="34"/>
+      <c r="WT57" s="34"/>
+      <c r="WU57" s="34"/>
+      <c r="WV57" s="34"/>
+      <c r="WW57" s="34"/>
+      <c r="WX57" s="34"/>
+      <c r="WY57" s="34"/>
+      <c r="WZ57" s="34"/>
+      <c r="XA57" s="34"/>
+      <c r="XB57" s="34"/>
+      <c r="XC57" s="34"/>
+      <c r="XD57" s="34"/>
+      <c r="XE57" s="34"/>
+      <c r="XF57" s="34"/>
+      <c r="XG57" s="34"/>
+      <c r="XH57" s="34"/>
+      <c r="XI57" s="34"/>
+      <c r="XJ57" s="34"/>
+      <c r="XK57" s="34"/>
+      <c r="XL57" s="34"/>
+      <c r="XM57" s="34"/>
+      <c r="XN57" s="34"/>
+      <c r="XO57" s="34"/>
+      <c r="XP57" s="34"/>
+      <c r="XQ57" s="34"/>
+      <c r="XR57" s="34"/>
+      <c r="XS57" s="34"/>
+      <c r="XT57" s="34"/>
+      <c r="XU57" s="34"/>
+      <c r="XV57" s="34"/>
+      <c r="XW57" s="34"/>
+      <c r="XX57" s="34"/>
+      <c r="XY57" s="34"/>
+      <c r="XZ57" s="34"/>
+      <c r="YA57" s="34"/>
+      <c r="YB57" s="34"/>
+      <c r="YC57" s="34"/>
+      <c r="YD57" s="34"/>
+      <c r="YE57" s="34"/>
+      <c r="YF57" s="34"/>
+      <c r="YG57" s="34"/>
+      <c r="YH57" s="34"/>
+      <c r="YI57" s="34"/>
+      <c r="YJ57" s="34"/>
+      <c r="YK57" s="34"/>
+      <c r="YL57" s="34"/>
+      <c r="YM57" s="34"/>
+      <c r="YN57" s="34"/>
+      <c r="YO57" s="34"/>
+      <c r="YP57" s="34"/>
+      <c r="YQ57" s="34"/>
+      <c r="YR57" s="34"/>
+      <c r="YS57" s="34"/>
+      <c r="YT57" s="34"/>
+      <c r="YU57" s="34"/>
+      <c r="YV57" s="34"/>
+      <c r="YW57" s="34"/>
+      <c r="YX57" s="34"/>
+      <c r="YY57" s="34"/>
+      <c r="YZ57" s="34"/>
+      <c r="ZA57" s="34"/>
+      <c r="ZB57" s="34"/>
+      <c r="ZC57" s="34"/>
+      <c r="ZD57" s="34"/>
+      <c r="ZE57" s="34"/>
+      <c r="ZF57" s="34"/>
+      <c r="ZG57" s="34"/>
+      <c r="ZH57" s="34"/>
+      <c r="ZI57" s="34"/>
+      <c r="ZJ57" s="34"/>
+      <c r="ZK57" s="34"/>
+      <c r="ZL57" s="34"/>
+      <c r="ZM57" s="34"/>
+      <c r="ZN57" s="34"/>
+      <c r="ZO57" s="34"/>
+      <c r="ZP57" s="34"/>
+      <c r="ZQ57" s="34"/>
+      <c r="ZR57" s="34"/>
+      <c r="ZS57" s="34"/>
+      <c r="ZT57" s="34"/>
+      <c r="ZU57" s="34"/>
+      <c r="ZV57" s="34"/>
+      <c r="ZW57" s="34"/>
+      <c r="ZX57" s="34"/>
+      <c r="ZY57" s="34"/>
+      <c r="ZZ57" s="34"/>
+      <c r="AAA57" s="34"/>
+      <c r="AAB57" s="34"/>
+      <c r="AAC57" s="34"/>
+      <c r="AAD57" s="34"/>
+      <c r="AAE57" s="34"/>
+      <c r="AAF57" s="34"/>
+      <c r="AAG57" s="34"/>
+      <c r="AAH57" s="34"/>
+      <c r="AAI57" s="34"/>
+      <c r="AAJ57" s="34"/>
+      <c r="AAK57" s="34"/>
+      <c r="AAL57" s="34"/>
+      <c r="AAM57" s="34"/>
+      <c r="AAN57" s="34"/>
+      <c r="AAO57" s="34"/>
+      <c r="AAP57" s="34"/>
+      <c r="AAQ57" s="34"/>
+      <c r="AAR57" s="34"/>
+      <c r="AAS57" s="34"/>
+      <c r="AAT57" s="34"/>
+      <c r="AAU57" s="34"/>
+      <c r="AAV57" s="34"/>
+      <c r="AAW57" s="34"/>
+      <c r="AAX57" s="34"/>
+      <c r="AAY57" s="34"/>
+      <c r="AAZ57" s="34"/>
+      <c r="ABA57" s="34"/>
+      <c r="ABB57" s="34"/>
+      <c r="ABC57" s="34"/>
+      <c r="ABD57" s="34"/>
+      <c r="ABE57" s="34"/>
+      <c r="ABF57" s="34"/>
+      <c r="ABG57" s="34"/>
+      <c r="ABH57" s="34"/>
+      <c r="ABI57" s="34"/>
+      <c r="ABJ57" s="34"/>
+      <c r="ABK57" s="34"/>
+      <c r="ABL57" s="34"/>
+      <c r="ABM57" s="34"/>
+      <c r="ABN57" s="34"/>
+      <c r="ABO57" s="34"/>
+      <c r="ABP57" s="34"/>
+      <c r="ABQ57" s="34"/>
+      <c r="ABR57" s="34"/>
+      <c r="ABS57" s="34"/>
+      <c r="ABT57" s="34"/>
+      <c r="ABU57" s="34"/>
+      <c r="ABV57" s="34"/>
+      <c r="ABW57" s="34"/>
+      <c r="ABX57" s="34"/>
+      <c r="ABY57" s="34"/>
+      <c r="ABZ57" s="34"/>
+      <c r="ACA57" s="34"/>
+      <c r="ACB57" s="34"/>
+      <c r="ACC57" s="34"/>
+      <c r="ACD57" s="34"/>
+      <c r="ACE57" s="34"/>
+      <c r="ACF57" s="34"/>
+      <c r="ACG57" s="34"/>
+      <c r="ACH57" s="34"/>
+      <c r="ACI57" s="34"/>
+      <c r="ACJ57" s="34"/>
+      <c r="ACK57" s="34"/>
+      <c r="ACL57" s="34"/>
+      <c r="ACM57" s="34"/>
+      <c r="ACN57" s="34"/>
+      <c r="ACO57" s="34"/>
+      <c r="ACP57" s="34"/>
+      <c r="ACQ57" s="34"/>
+      <c r="ACR57" s="34"/>
+      <c r="ACS57" s="34"/>
+      <c r="ACT57" s="34"/>
+      <c r="ACU57" s="34"/>
+      <c r="ACV57" s="34"/>
+      <c r="ACW57" s="34"/>
+      <c r="ACX57" s="34"/>
+      <c r="ACY57" s="34"/>
+      <c r="ACZ57" s="34"/>
+      <c r="ADA57" s="34"/>
+      <c r="ADB57" s="34"/>
+      <c r="ADC57" s="34"/>
+      <c r="ADD57" s="34"/>
+      <c r="ADE57" s="34"/>
+      <c r="ADF57" s="34"/>
+      <c r="ADG57" s="34"/>
+      <c r="ADH57" s="34"/>
+      <c r="ADI57" s="34"/>
+      <c r="ADJ57" s="34"/>
+      <c r="ADK57" s="34"/>
+      <c r="ADL57" s="34"/>
+      <c r="ADM57" s="34"/>
+      <c r="ADN57" s="34"/>
+      <c r="ADO57" s="34"/>
+      <c r="ADP57" s="34"/>
+      <c r="ADQ57" s="34"/>
+      <c r="ADR57" s="34"/>
+      <c r="ADS57" s="34"/>
+      <c r="ADT57" s="34"/>
+      <c r="ADU57" s="34"/>
+      <c r="ADV57" s="34"/>
+      <c r="ADW57" s="34"/>
+      <c r="ADX57" s="34"/>
+      <c r="ADY57" s="34"/>
+      <c r="ADZ57" s="34"/>
+      <c r="AEA57" s="34"/>
+      <c r="AEB57" s="34"/>
+      <c r="AEC57" s="34"/>
+      <c r="AED57" s="34"/>
+      <c r="AEE57" s="34"/>
+      <c r="AEF57" s="34"/>
+      <c r="AEG57" s="34"/>
+      <c r="AEH57" s="34"/>
+      <c r="AEI57" s="34"/>
+      <c r="AEJ57" s="34"/>
+      <c r="AEK57" s="34"/>
+      <c r="AEL57" s="34"/>
+      <c r="AEM57" s="34"/>
+      <c r="AEN57" s="34"/>
+      <c r="AEO57" s="34"/>
+      <c r="AEP57" s="34"/>
+      <c r="AEQ57" s="34"/>
+      <c r="AER57" s="34"/>
+      <c r="AES57" s="34"/>
+      <c r="AET57" s="34"/>
+      <c r="AEU57" s="34"/>
+      <c r="AEV57" s="34"/>
+      <c r="AEW57" s="34"/>
+      <c r="AEX57" s="34"/>
+      <c r="AEY57" s="34"/>
+      <c r="AEZ57" s="34"/>
+      <c r="AFA57" s="34"/>
+      <c r="AFB57" s="34"/>
+      <c r="AFC57" s="34"/>
+      <c r="AFD57" s="34"/>
+      <c r="AFE57" s="34"/>
+      <c r="AFF57" s="34"/>
+      <c r="AFG57" s="34"/>
+      <c r="AFH57" s="34"/>
+      <c r="AFI57" s="34"/>
+      <c r="AFJ57" s="34"/>
+      <c r="AFK57" s="34"/>
+      <c r="AFL57" s="34"/>
+      <c r="AFM57" s="34"/>
+      <c r="AFN57" s="34"/>
+      <c r="AFO57" s="34"/>
+      <c r="AFP57" s="34"/>
+      <c r="AFQ57" s="34"/>
+      <c r="AFR57" s="34"/>
+      <c r="AFS57" s="34"/>
+      <c r="AFT57" s="34"/>
+      <c r="AFU57" s="34"/>
+      <c r="AFV57" s="34"/>
+      <c r="AFW57" s="34"/>
+      <c r="AFX57" s="34"/>
+      <c r="AFY57" s="34"/>
+      <c r="AFZ57" s="34"/>
+      <c r="AGA57" s="34"/>
+      <c r="AGB57" s="34"/>
+      <c r="AGC57" s="34"/>
+      <c r="AGD57" s="34"/>
+      <c r="AGE57" s="34"/>
+      <c r="AGF57" s="34"/>
+      <c r="AGG57" s="34"/>
+      <c r="AGH57" s="34"/>
+      <c r="AGI57" s="34"/>
+      <c r="AGJ57" s="34"/>
+      <c r="AGK57" s="34"/>
+      <c r="AGL57" s="34"/>
+      <c r="AGM57" s="34"/>
+      <c r="AGN57" s="34"/>
+      <c r="AGO57" s="34"/>
+      <c r="AGP57" s="34"/>
+      <c r="AGQ57" s="34"/>
+      <c r="AGR57" s="34"/>
+      <c r="AGS57" s="34"/>
+      <c r="AGT57" s="34"/>
+      <c r="AGU57" s="34"/>
+      <c r="AGV57" s="34"/>
+      <c r="AGW57" s="34"/>
+      <c r="AGX57" s="34"/>
+      <c r="AGY57" s="34"/>
+      <c r="AGZ57" s="34"/>
+      <c r="AHA57" s="34"/>
+      <c r="AHB57" s="34"/>
+      <c r="AHC57" s="34"/>
+      <c r="AHD57" s="34"/>
+      <c r="AHE57" s="34"/>
+      <c r="AHF57" s="34"/>
+      <c r="AHG57" s="34"/>
+      <c r="AHH57" s="34"/>
+      <c r="AHI57" s="34"/>
+      <c r="AHJ57" s="34"/>
+      <c r="AHK57" s="34"/>
+      <c r="AHL57" s="34"/>
+      <c r="AHM57" s="34"/>
+      <c r="AHN57" s="34"/>
+      <c r="AHO57" s="34"/>
       <c r="AHP57" s="33" t="s">
         <v>27</v>
       </c>
@@ -35679,932 +35711,932 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:11842" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11842" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="41" t="s">
+      <c r="B58" s="54"/>
+      <c r="C58" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="46" t="s">
+      <c r="D58" s="45" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:11842" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="36" t="s">
+    <row r="59" spans="1:11842" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="54" t="s">
+      <c r="B59" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="40"/>
-      <c r="D59" s="56" t="s">
+      <c r="C59" s="78"/>
+      <c r="D59" s="58" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:11842" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11842" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="55"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="35"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="35"/>
-      <c r="P60" s="35"/>
-      <c r="Q60" s="35"/>
-      <c r="R60" s="35"/>
-      <c r="S60" s="35"/>
-      <c r="T60" s="35"/>
-      <c r="U60" s="35"/>
-      <c r="V60" s="35"/>
-      <c r="W60" s="35"/>
-      <c r="X60" s="35"/>
-      <c r="Y60" s="35"/>
-      <c r="Z60" s="35"/>
-      <c r="AA60" s="35"/>
-      <c r="AB60" s="35"/>
-      <c r="AC60" s="35"/>
-      <c r="AD60" s="35"/>
-      <c r="AE60" s="35"/>
-      <c r="AF60" s="35"/>
-      <c r="AG60" s="35"/>
-      <c r="AH60" s="35"/>
-      <c r="AI60" s="35"/>
-      <c r="AJ60" s="35"/>
-      <c r="AK60" s="35"/>
-      <c r="AL60" s="35"/>
-      <c r="AM60" s="35"/>
-      <c r="AN60" s="35"/>
-      <c r="AO60" s="35"/>
-      <c r="AP60" s="35"/>
-      <c r="AQ60" s="35"/>
-      <c r="AR60" s="35"/>
-      <c r="AS60" s="35"/>
-      <c r="AT60" s="35"/>
-      <c r="AU60" s="35"/>
-      <c r="AV60" s="35"/>
-      <c r="AW60" s="35"/>
-      <c r="AX60" s="35"/>
-      <c r="AY60" s="35"/>
-      <c r="AZ60" s="35"/>
-      <c r="BA60" s="35"/>
-      <c r="BB60" s="35"/>
-      <c r="BC60" s="35"/>
-      <c r="BD60" s="35"/>
-      <c r="BE60" s="35"/>
-      <c r="BF60" s="35"/>
-      <c r="BG60" s="35"/>
-      <c r="BH60" s="35"/>
-      <c r="BI60" s="35"/>
-      <c r="BJ60" s="35"/>
-      <c r="BK60" s="35"/>
-      <c r="BL60" s="35"/>
-      <c r="BM60" s="35"/>
-      <c r="BN60" s="35"/>
-      <c r="BO60" s="35"/>
-      <c r="BP60" s="35"/>
-      <c r="BQ60" s="35"/>
-      <c r="BR60" s="35"/>
-      <c r="BS60" s="35"/>
-      <c r="BT60" s="35"/>
-      <c r="BU60" s="35"/>
-      <c r="BV60" s="35"/>
-      <c r="BW60" s="35"/>
-      <c r="BX60" s="35"/>
-      <c r="BY60" s="35"/>
-      <c r="BZ60" s="35"/>
-      <c r="CA60" s="35"/>
-      <c r="CB60" s="35"/>
-      <c r="CC60" s="35"/>
-      <c r="CD60" s="35"/>
-      <c r="CE60" s="35"/>
-      <c r="CF60" s="35"/>
-      <c r="CG60" s="35"/>
-      <c r="CH60" s="35"/>
-      <c r="CI60" s="35"/>
-      <c r="CJ60" s="35"/>
-      <c r="CK60" s="35"/>
-      <c r="CL60" s="35"/>
-      <c r="CM60" s="35"/>
-      <c r="CN60" s="35"/>
-      <c r="CO60" s="35"/>
-      <c r="CP60" s="35"/>
-      <c r="CQ60" s="35"/>
-      <c r="CR60" s="35"/>
-      <c r="CS60" s="35"/>
-      <c r="CT60" s="35"/>
-      <c r="CU60" s="35"/>
-      <c r="CV60" s="35"/>
-      <c r="CW60" s="35"/>
-      <c r="CX60" s="35"/>
-      <c r="CY60" s="35"/>
-      <c r="CZ60" s="35"/>
-      <c r="DA60" s="35"/>
-      <c r="DB60" s="35"/>
-      <c r="DC60" s="35"/>
-      <c r="DD60" s="35"/>
-      <c r="DE60" s="35"/>
-      <c r="DF60" s="35"/>
-      <c r="DG60" s="35"/>
-      <c r="DH60" s="35"/>
-      <c r="DI60" s="35"/>
-      <c r="DJ60" s="35"/>
-      <c r="DK60" s="35"/>
-      <c r="DL60" s="35"/>
-      <c r="DM60" s="35"/>
-      <c r="DN60" s="35"/>
-      <c r="DO60" s="35"/>
-      <c r="DP60" s="35"/>
-      <c r="DQ60" s="35"/>
-      <c r="DR60" s="35"/>
-      <c r="DS60" s="35"/>
-      <c r="DT60" s="35"/>
-      <c r="DU60" s="35"/>
-      <c r="DV60" s="35"/>
-      <c r="DW60" s="35"/>
-      <c r="DX60" s="35"/>
-      <c r="DY60" s="35"/>
-      <c r="DZ60" s="35"/>
-      <c r="EA60" s="35"/>
-      <c r="EB60" s="35"/>
-      <c r="EC60" s="35"/>
-      <c r="ED60" s="35"/>
-      <c r="EE60" s="35"/>
-      <c r="EF60" s="35"/>
-      <c r="EG60" s="35"/>
-      <c r="EH60" s="35"/>
-      <c r="EI60" s="35"/>
-      <c r="EJ60" s="35"/>
-      <c r="EK60" s="35"/>
-      <c r="EL60" s="35"/>
-      <c r="EM60" s="35"/>
-      <c r="EN60" s="35"/>
-      <c r="EO60" s="35"/>
-      <c r="EP60" s="35"/>
-      <c r="EQ60" s="35"/>
-      <c r="ER60" s="35"/>
-      <c r="ES60" s="35"/>
-      <c r="ET60" s="35"/>
-      <c r="EU60" s="35"/>
-      <c r="EV60" s="35"/>
-      <c r="EW60" s="35"/>
-      <c r="EX60" s="35"/>
-      <c r="EY60" s="35"/>
-      <c r="EZ60" s="35"/>
-      <c r="FA60" s="35"/>
-      <c r="FB60" s="35"/>
-      <c r="FC60" s="35"/>
-      <c r="FD60" s="35"/>
-      <c r="FE60" s="35"/>
-      <c r="FF60" s="35"/>
-      <c r="FG60" s="35"/>
-      <c r="FH60" s="35"/>
-      <c r="FI60" s="35"/>
-      <c r="FJ60" s="35"/>
-      <c r="FK60" s="35"/>
-      <c r="FL60" s="35"/>
-      <c r="FM60" s="35"/>
-      <c r="FN60" s="35"/>
-      <c r="FO60" s="35"/>
-      <c r="FP60" s="35"/>
-      <c r="FQ60" s="35"/>
-      <c r="FR60" s="35"/>
-      <c r="FS60" s="35"/>
-      <c r="FT60" s="35"/>
-      <c r="FU60" s="35"/>
-      <c r="FV60" s="35"/>
-      <c r="FW60" s="35"/>
-      <c r="FX60" s="35"/>
-      <c r="FY60" s="35"/>
-      <c r="FZ60" s="35"/>
-      <c r="GA60" s="35"/>
-      <c r="GB60" s="35"/>
-      <c r="GC60" s="35"/>
-      <c r="GD60" s="35"/>
-      <c r="GE60" s="35"/>
-      <c r="GF60" s="35"/>
-      <c r="GG60" s="35"/>
-      <c r="GH60" s="35"/>
-      <c r="GI60" s="35"/>
-      <c r="GJ60" s="35"/>
-      <c r="GK60" s="35"/>
-      <c r="GL60" s="35"/>
-      <c r="GM60" s="35"/>
-      <c r="GN60" s="35"/>
-      <c r="GO60" s="35"/>
-      <c r="GP60" s="35"/>
-      <c r="GQ60" s="35"/>
-      <c r="GR60" s="35"/>
-      <c r="GS60" s="35"/>
-      <c r="GT60" s="35"/>
-      <c r="GU60" s="35"/>
-      <c r="GV60" s="35"/>
-      <c r="GW60" s="35"/>
-      <c r="GX60" s="35"/>
-      <c r="GY60" s="35"/>
-      <c r="GZ60" s="35"/>
-      <c r="HA60" s="35"/>
-      <c r="HB60" s="35"/>
-      <c r="HC60" s="35"/>
-      <c r="HD60" s="35"/>
-      <c r="HE60" s="35"/>
-      <c r="HF60" s="35"/>
-      <c r="HG60" s="35"/>
-      <c r="HH60" s="35"/>
-      <c r="HI60" s="35"/>
-      <c r="HJ60" s="35"/>
-      <c r="HK60" s="35"/>
-      <c r="HL60" s="35"/>
-      <c r="HM60" s="35"/>
-      <c r="HN60" s="35"/>
-      <c r="HO60" s="35"/>
-      <c r="HP60" s="35"/>
-      <c r="HQ60" s="35"/>
-      <c r="HR60" s="35"/>
-      <c r="HS60" s="35"/>
-      <c r="HT60" s="35"/>
-      <c r="HU60" s="35"/>
-      <c r="HV60" s="35"/>
-      <c r="HW60" s="35"/>
-      <c r="HX60" s="35"/>
-      <c r="HY60" s="35"/>
-      <c r="HZ60" s="35"/>
-      <c r="IA60" s="35"/>
-      <c r="IB60" s="35"/>
-      <c r="IC60" s="35"/>
-      <c r="ID60" s="35"/>
-      <c r="IE60" s="35"/>
-      <c r="IF60" s="35"/>
-      <c r="IG60" s="35"/>
-      <c r="IH60" s="35"/>
-      <c r="II60" s="35"/>
-      <c r="IJ60" s="35"/>
-      <c r="IK60" s="35"/>
-      <c r="IL60" s="35"/>
-      <c r="IM60" s="35"/>
-      <c r="IN60" s="35"/>
-      <c r="IO60" s="35"/>
-      <c r="IP60" s="35"/>
-      <c r="IQ60" s="35"/>
-      <c r="IR60" s="35"/>
-      <c r="IS60" s="35"/>
-      <c r="IT60" s="35"/>
-      <c r="IU60" s="35"/>
-      <c r="IV60" s="35"/>
-      <c r="IW60" s="35"/>
-      <c r="IX60" s="35"/>
-      <c r="IY60" s="35"/>
-      <c r="IZ60" s="35"/>
-      <c r="JA60" s="35"/>
-      <c r="JB60" s="35"/>
-      <c r="JC60" s="35"/>
-      <c r="JD60" s="35"/>
-      <c r="JE60" s="35"/>
-      <c r="JF60" s="35"/>
-      <c r="JG60" s="35"/>
-      <c r="JH60" s="35"/>
-      <c r="JI60" s="35"/>
-      <c r="JJ60" s="35"/>
-      <c r="JK60" s="35"/>
-      <c r="JL60" s="35"/>
-      <c r="JM60" s="35"/>
-      <c r="JN60" s="35"/>
-      <c r="JO60" s="35"/>
-      <c r="JP60" s="35"/>
-      <c r="JQ60" s="35"/>
-      <c r="JR60" s="35"/>
-      <c r="JS60" s="35"/>
-      <c r="JT60" s="35"/>
-      <c r="JU60" s="35"/>
-      <c r="JV60" s="35"/>
-      <c r="JW60" s="35"/>
-      <c r="JX60" s="35"/>
-      <c r="JY60" s="35"/>
-      <c r="JZ60" s="35"/>
-      <c r="KA60" s="35"/>
-      <c r="KB60" s="35"/>
-      <c r="KC60" s="35"/>
-      <c r="KD60" s="35"/>
-      <c r="KE60" s="35"/>
-      <c r="KF60" s="35"/>
-      <c r="KG60" s="35"/>
-      <c r="KH60" s="35"/>
-      <c r="KI60" s="35"/>
-      <c r="KJ60" s="35"/>
-      <c r="KK60" s="35"/>
-      <c r="KL60" s="35"/>
-      <c r="KM60" s="35"/>
-      <c r="KN60" s="35"/>
-      <c r="KO60" s="35"/>
-      <c r="KP60" s="35"/>
-      <c r="KQ60" s="35"/>
-      <c r="KR60" s="35"/>
-      <c r="KS60" s="35"/>
-      <c r="KT60" s="35"/>
-      <c r="KU60" s="35"/>
-      <c r="KV60" s="35"/>
-      <c r="KW60" s="35"/>
-      <c r="KX60" s="35"/>
-      <c r="KY60" s="35"/>
-      <c r="KZ60" s="35"/>
-      <c r="LA60" s="35"/>
-      <c r="LB60" s="35"/>
-      <c r="LC60" s="35"/>
-      <c r="LD60" s="35"/>
-      <c r="LE60" s="35"/>
-      <c r="LF60" s="35"/>
-      <c r="LG60" s="35"/>
-      <c r="LH60" s="35"/>
-      <c r="LI60" s="35"/>
-      <c r="LJ60" s="35"/>
-      <c r="LK60" s="35"/>
-      <c r="LL60" s="35"/>
-      <c r="LM60" s="35"/>
-      <c r="LN60" s="35"/>
-      <c r="LO60" s="35"/>
-      <c r="LP60" s="35"/>
-      <c r="LQ60" s="35"/>
-      <c r="LR60" s="35"/>
-      <c r="LS60" s="35"/>
-      <c r="LT60" s="35"/>
-      <c r="LU60" s="35"/>
-      <c r="LV60" s="35"/>
-      <c r="LW60" s="35"/>
-      <c r="LX60" s="35"/>
-      <c r="LY60" s="35"/>
-      <c r="LZ60" s="35"/>
-      <c r="MA60" s="35"/>
-      <c r="MB60" s="35"/>
-      <c r="MC60" s="35"/>
-      <c r="MD60" s="35"/>
-      <c r="ME60" s="35"/>
-      <c r="MF60" s="35"/>
-      <c r="MG60" s="35"/>
-      <c r="MH60" s="35"/>
-      <c r="MI60" s="35"/>
-      <c r="MJ60" s="35"/>
-      <c r="MK60" s="35"/>
-      <c r="ML60" s="35"/>
-      <c r="MM60" s="35"/>
-      <c r="MN60" s="35"/>
-      <c r="MO60" s="35"/>
-      <c r="MP60" s="35"/>
-      <c r="MQ60" s="35"/>
-      <c r="MR60" s="35"/>
-      <c r="MS60" s="35"/>
-      <c r="MT60" s="35"/>
-      <c r="MU60" s="35"/>
-      <c r="MV60" s="35"/>
-      <c r="MW60" s="35"/>
-      <c r="MX60" s="35"/>
-      <c r="MY60" s="35"/>
-      <c r="MZ60" s="35"/>
-      <c r="NA60" s="35"/>
-      <c r="NB60" s="35"/>
-      <c r="NC60" s="35"/>
-      <c r="ND60" s="35"/>
-      <c r="NE60" s="35"/>
-      <c r="NF60" s="35"/>
-      <c r="NG60" s="35"/>
-      <c r="NH60" s="35"/>
-      <c r="NI60" s="35"/>
-      <c r="NJ60" s="35"/>
-      <c r="NK60" s="35"/>
-      <c r="NL60" s="35"/>
-      <c r="NM60" s="35"/>
-      <c r="NN60" s="35"/>
-      <c r="NO60" s="35"/>
-      <c r="NP60" s="35"/>
-      <c r="NQ60" s="35"/>
-      <c r="NR60" s="35"/>
-      <c r="NS60" s="35"/>
-      <c r="NT60" s="35"/>
-      <c r="NU60" s="35"/>
-      <c r="NV60" s="35"/>
-      <c r="NW60" s="35"/>
-      <c r="NX60" s="35"/>
-      <c r="NY60" s="35"/>
-      <c r="NZ60" s="35"/>
-      <c r="OA60" s="35"/>
-      <c r="OB60" s="35"/>
-      <c r="OC60" s="35"/>
-      <c r="OD60" s="35"/>
-      <c r="OE60" s="35"/>
-      <c r="OF60" s="35"/>
-      <c r="OG60" s="35"/>
-      <c r="OH60" s="35"/>
-      <c r="OI60" s="35"/>
-      <c r="OJ60" s="35"/>
-      <c r="OK60" s="35"/>
-      <c r="OL60" s="35"/>
-      <c r="OM60" s="35"/>
-      <c r="ON60" s="35"/>
-      <c r="OO60" s="35"/>
-      <c r="OP60" s="35"/>
-      <c r="OQ60" s="35"/>
-      <c r="OR60" s="35"/>
-      <c r="OS60" s="35"/>
-      <c r="OT60" s="35"/>
-      <c r="OU60" s="35"/>
-      <c r="OV60" s="35"/>
-      <c r="OW60" s="35"/>
-      <c r="OX60" s="35"/>
-      <c r="OY60" s="35"/>
-      <c r="OZ60" s="35"/>
-      <c r="PA60" s="35"/>
-      <c r="PB60" s="35"/>
-      <c r="PC60" s="35"/>
-      <c r="PD60" s="35"/>
-      <c r="PE60" s="35"/>
-      <c r="PF60" s="35"/>
-      <c r="PG60" s="35"/>
-      <c r="PH60" s="35"/>
-      <c r="PI60" s="35"/>
-      <c r="PJ60" s="35"/>
-      <c r="PK60" s="35"/>
-      <c r="PL60" s="35"/>
-      <c r="PM60" s="35"/>
-      <c r="PN60" s="35"/>
-      <c r="PO60" s="35"/>
-      <c r="PP60" s="35"/>
-      <c r="PQ60" s="35"/>
-      <c r="PR60" s="35"/>
-      <c r="PS60" s="35"/>
-      <c r="PT60" s="35"/>
-      <c r="PU60" s="35"/>
-      <c r="PV60" s="35"/>
-      <c r="PW60" s="35"/>
-      <c r="PX60" s="35"/>
-      <c r="PY60" s="35"/>
-      <c r="PZ60" s="35"/>
-      <c r="QA60" s="35"/>
-      <c r="QB60" s="35"/>
-      <c r="QC60" s="35"/>
-      <c r="QD60" s="35"/>
-      <c r="QE60" s="35"/>
-      <c r="QF60" s="35"/>
-      <c r="QG60" s="35"/>
-      <c r="QH60" s="35"/>
-      <c r="QI60" s="35"/>
-      <c r="QJ60" s="35"/>
-      <c r="QK60" s="35"/>
-      <c r="QL60" s="35"/>
-      <c r="QM60" s="35"/>
-      <c r="QN60" s="35"/>
-      <c r="QO60" s="35"/>
-      <c r="QP60" s="35"/>
-      <c r="QQ60" s="35"/>
-      <c r="QR60" s="35"/>
-      <c r="QS60" s="35"/>
-      <c r="QT60" s="35"/>
-      <c r="QU60" s="35"/>
-      <c r="QV60" s="35"/>
-      <c r="QW60" s="35"/>
-      <c r="QX60" s="35"/>
-      <c r="QY60" s="35"/>
-      <c r="QZ60" s="35"/>
-      <c r="RA60" s="35"/>
-      <c r="RB60" s="35"/>
-      <c r="RC60" s="35"/>
-      <c r="RD60" s="35"/>
-      <c r="RE60" s="35"/>
-      <c r="RF60" s="35"/>
-      <c r="RG60" s="35"/>
-      <c r="RH60" s="35"/>
-      <c r="RI60" s="35"/>
-      <c r="RJ60" s="35"/>
-      <c r="RK60" s="35"/>
-      <c r="RL60" s="35"/>
-      <c r="RM60" s="35"/>
-      <c r="RN60" s="35"/>
-      <c r="RO60" s="35"/>
-      <c r="RP60" s="35"/>
-      <c r="RQ60" s="35"/>
-      <c r="RR60" s="35"/>
-      <c r="RS60" s="35"/>
-      <c r="RT60" s="35"/>
-      <c r="RU60" s="35"/>
-      <c r="RV60" s="35"/>
-      <c r="RW60" s="35"/>
-      <c r="RX60" s="35"/>
-      <c r="RY60" s="35"/>
-      <c r="RZ60" s="35"/>
-      <c r="SA60" s="35"/>
-      <c r="SB60" s="35"/>
-      <c r="SC60" s="35"/>
-      <c r="SD60" s="35"/>
-      <c r="SE60" s="35"/>
-      <c r="SF60" s="35"/>
-      <c r="SG60" s="35"/>
-      <c r="SH60" s="35"/>
-      <c r="SI60" s="35"/>
-      <c r="SJ60" s="35"/>
-      <c r="SK60" s="35"/>
-      <c r="SL60" s="35"/>
-      <c r="SM60" s="35"/>
-      <c r="SN60" s="35"/>
-      <c r="SO60" s="35"/>
-      <c r="SP60" s="35"/>
-      <c r="SQ60" s="35"/>
-      <c r="SR60" s="35"/>
-      <c r="SS60" s="35"/>
-      <c r="ST60" s="35"/>
-      <c r="SU60" s="35"/>
-      <c r="SV60" s="35"/>
-      <c r="SW60" s="35"/>
-      <c r="SX60" s="35"/>
-      <c r="SY60" s="35"/>
-      <c r="SZ60" s="35"/>
-      <c r="TA60" s="35"/>
-      <c r="TB60" s="35"/>
-      <c r="TC60" s="35"/>
-      <c r="TD60" s="35"/>
-      <c r="TE60" s="35"/>
-      <c r="TF60" s="35"/>
-      <c r="TG60" s="35"/>
-      <c r="TH60" s="35"/>
-      <c r="TI60" s="35"/>
-      <c r="TJ60" s="35"/>
-      <c r="TK60" s="35"/>
-      <c r="TL60" s="35"/>
-      <c r="TM60" s="35"/>
-      <c r="TN60" s="35"/>
-      <c r="TO60" s="35"/>
-      <c r="TP60" s="35"/>
-      <c r="TQ60" s="35"/>
-      <c r="TR60" s="35"/>
-      <c r="TS60" s="35"/>
-      <c r="TT60" s="35"/>
-      <c r="TU60" s="35"/>
-      <c r="TV60" s="35"/>
-      <c r="TW60" s="35"/>
-      <c r="TX60" s="35"/>
-      <c r="TY60" s="35"/>
-      <c r="TZ60" s="35"/>
-      <c r="UA60" s="35"/>
-      <c r="UB60" s="35"/>
-      <c r="UC60" s="35"/>
-      <c r="UD60" s="35"/>
-      <c r="UE60" s="35"/>
-      <c r="UF60" s="35"/>
-      <c r="UG60" s="35"/>
-      <c r="UH60" s="35"/>
-      <c r="UI60" s="35"/>
-      <c r="UJ60" s="35"/>
-      <c r="UK60" s="35"/>
-      <c r="UL60" s="35"/>
-      <c r="UM60" s="35"/>
-      <c r="UN60" s="35"/>
-      <c r="UO60" s="35"/>
-      <c r="UP60" s="35"/>
-      <c r="UQ60" s="35"/>
-      <c r="UR60" s="35"/>
-      <c r="US60" s="35"/>
-      <c r="UT60" s="35"/>
-      <c r="UU60" s="35"/>
-      <c r="UV60" s="35"/>
-      <c r="UW60" s="35"/>
-      <c r="UX60" s="35"/>
-      <c r="UY60" s="35"/>
-      <c r="UZ60" s="35"/>
-      <c r="VA60" s="35"/>
-      <c r="VB60" s="35"/>
-      <c r="VC60" s="35"/>
-      <c r="VD60" s="35"/>
-      <c r="VE60" s="35"/>
-      <c r="VF60" s="35"/>
-      <c r="VG60" s="35"/>
-      <c r="VH60" s="35"/>
-      <c r="VI60" s="35"/>
-      <c r="VJ60" s="35"/>
-      <c r="VK60" s="35"/>
-      <c r="VL60" s="35"/>
-      <c r="VM60" s="35"/>
-      <c r="VN60" s="35"/>
-      <c r="VO60" s="35"/>
-      <c r="VP60" s="35"/>
-      <c r="VQ60" s="35"/>
-      <c r="VR60" s="35"/>
-      <c r="VS60" s="35"/>
-      <c r="VT60" s="35"/>
-      <c r="VU60" s="35"/>
-      <c r="VV60" s="35"/>
-      <c r="VW60" s="35"/>
-      <c r="VX60" s="35"/>
-      <c r="VY60" s="35"/>
-      <c r="VZ60" s="35"/>
-      <c r="WA60" s="35"/>
-      <c r="WB60" s="35"/>
-      <c r="WC60" s="35"/>
-      <c r="WD60" s="35"/>
-      <c r="WE60" s="35"/>
-      <c r="WF60" s="35"/>
-      <c r="WG60" s="35"/>
-      <c r="WH60" s="35"/>
-      <c r="WI60" s="35"/>
-      <c r="WJ60" s="35"/>
-      <c r="WK60" s="35"/>
-      <c r="WL60" s="35"/>
-      <c r="WM60" s="35"/>
-      <c r="WN60" s="35"/>
-      <c r="WO60" s="35"/>
-      <c r="WP60" s="35"/>
-      <c r="WQ60" s="35"/>
-      <c r="WR60" s="35"/>
-      <c r="WS60" s="35"/>
-      <c r="WT60" s="35"/>
-      <c r="WU60" s="35"/>
-      <c r="WV60" s="35"/>
-      <c r="WW60" s="35"/>
-      <c r="WX60" s="35"/>
-      <c r="WY60" s="35"/>
-      <c r="WZ60" s="35"/>
-      <c r="XA60" s="35"/>
-      <c r="XB60" s="35"/>
-      <c r="XC60" s="35"/>
-      <c r="XD60" s="35"/>
-      <c r="XE60" s="35"/>
-      <c r="XF60" s="35"/>
-      <c r="XG60" s="35"/>
-      <c r="XH60" s="35"/>
-      <c r="XI60" s="35"/>
-      <c r="XJ60" s="35"/>
-      <c r="XK60" s="35"/>
-      <c r="XL60" s="35"/>
-      <c r="XM60" s="35"/>
-      <c r="XN60" s="35"/>
-      <c r="XO60" s="35"/>
-      <c r="XP60" s="35"/>
-      <c r="XQ60" s="35"/>
-      <c r="XR60" s="35"/>
-      <c r="XS60" s="35"/>
-      <c r="XT60" s="35"/>
-      <c r="XU60" s="35"/>
-      <c r="XV60" s="35"/>
-      <c r="XW60" s="35"/>
-      <c r="XX60" s="35"/>
-      <c r="XY60" s="35"/>
-      <c r="XZ60" s="35"/>
-      <c r="YA60" s="35"/>
-      <c r="YB60" s="35"/>
-      <c r="YC60" s="35"/>
-      <c r="YD60" s="35"/>
-      <c r="YE60" s="35"/>
-      <c r="YF60" s="35"/>
-      <c r="YG60" s="35"/>
-      <c r="YH60" s="35"/>
-      <c r="YI60" s="35"/>
-      <c r="YJ60" s="35"/>
-      <c r="YK60" s="35"/>
-      <c r="YL60" s="35"/>
-      <c r="YM60" s="35"/>
-      <c r="YN60" s="35"/>
-      <c r="YO60" s="35"/>
-      <c r="YP60" s="35"/>
-      <c r="YQ60" s="35"/>
-      <c r="YR60" s="35"/>
-      <c r="YS60" s="35"/>
-      <c r="YT60" s="35"/>
-      <c r="YU60" s="35"/>
-      <c r="YV60" s="35"/>
-      <c r="YW60" s="35"/>
-      <c r="YX60" s="35"/>
-      <c r="YY60" s="35"/>
-      <c r="YZ60" s="35"/>
-      <c r="ZA60" s="35"/>
-      <c r="ZB60" s="35"/>
-      <c r="ZC60" s="35"/>
-      <c r="ZD60" s="35"/>
-      <c r="ZE60" s="35"/>
-      <c r="ZF60" s="35"/>
-      <c r="ZG60" s="35"/>
-      <c r="ZH60" s="35"/>
-      <c r="ZI60" s="35"/>
-      <c r="ZJ60" s="35"/>
-      <c r="ZK60" s="35"/>
-      <c r="ZL60" s="35"/>
-      <c r="ZM60" s="35"/>
-      <c r="ZN60" s="35"/>
-      <c r="ZO60" s="35"/>
-      <c r="ZP60" s="35"/>
-      <c r="ZQ60" s="35"/>
-      <c r="ZR60" s="35"/>
-      <c r="ZS60" s="35"/>
-      <c r="ZT60" s="35"/>
-      <c r="ZU60" s="35"/>
-      <c r="ZV60" s="35"/>
-      <c r="ZW60" s="35"/>
-      <c r="ZX60" s="35"/>
-      <c r="ZY60" s="35"/>
-      <c r="ZZ60" s="35"/>
-      <c r="AAA60" s="35"/>
-      <c r="AAB60" s="35"/>
-      <c r="AAC60" s="35"/>
-      <c r="AAD60" s="35"/>
-      <c r="AAE60" s="35"/>
-      <c r="AAF60" s="35"/>
-      <c r="AAG60" s="35"/>
-      <c r="AAH60" s="35"/>
-      <c r="AAI60" s="35"/>
-      <c r="AAJ60" s="35"/>
-      <c r="AAK60" s="35"/>
-      <c r="AAL60" s="35"/>
-      <c r="AAM60" s="35"/>
-      <c r="AAN60" s="35"/>
-      <c r="AAO60" s="35"/>
-      <c r="AAP60" s="35"/>
-      <c r="AAQ60" s="35"/>
-      <c r="AAR60" s="35"/>
-      <c r="AAS60" s="35"/>
-      <c r="AAT60" s="35"/>
-      <c r="AAU60" s="35"/>
-      <c r="AAV60" s="35"/>
-      <c r="AAW60" s="35"/>
-      <c r="AAX60" s="35"/>
-      <c r="AAY60" s="35"/>
-      <c r="AAZ60" s="35"/>
-      <c r="ABA60" s="35"/>
-      <c r="ABB60" s="35"/>
-      <c r="ABC60" s="35"/>
-      <c r="ABD60" s="35"/>
-      <c r="ABE60" s="35"/>
-      <c r="ABF60" s="35"/>
-      <c r="ABG60" s="35"/>
-      <c r="ABH60" s="35"/>
-      <c r="ABI60" s="35"/>
-      <c r="ABJ60" s="35"/>
-      <c r="ABK60" s="35"/>
-      <c r="ABL60" s="35"/>
-      <c r="ABM60" s="35"/>
-      <c r="ABN60" s="35"/>
-      <c r="ABO60" s="35"/>
-      <c r="ABP60" s="35"/>
-      <c r="ABQ60" s="35"/>
-      <c r="ABR60" s="35"/>
-      <c r="ABS60" s="35"/>
-      <c r="ABT60" s="35"/>
-      <c r="ABU60" s="35"/>
-      <c r="ABV60" s="35"/>
-      <c r="ABW60" s="35"/>
-      <c r="ABX60" s="35"/>
-      <c r="ABY60" s="35"/>
-      <c r="ABZ60" s="35"/>
-      <c r="ACA60" s="35"/>
-      <c r="ACB60" s="35"/>
-      <c r="ACC60" s="35"/>
-      <c r="ACD60" s="35"/>
-      <c r="ACE60" s="35"/>
-      <c r="ACF60" s="35"/>
-      <c r="ACG60" s="35"/>
-      <c r="ACH60" s="35"/>
-      <c r="ACI60" s="35"/>
-      <c r="ACJ60" s="35"/>
-      <c r="ACK60" s="35"/>
-      <c r="ACL60" s="35"/>
-      <c r="ACM60" s="35"/>
-      <c r="ACN60" s="35"/>
-      <c r="ACO60" s="35"/>
-      <c r="ACP60" s="35"/>
-      <c r="ACQ60" s="35"/>
-      <c r="ACR60" s="35"/>
-      <c r="ACS60" s="35"/>
-      <c r="ACT60" s="35"/>
-      <c r="ACU60" s="35"/>
-      <c r="ACV60" s="35"/>
-      <c r="ACW60" s="35"/>
-      <c r="ACX60" s="35"/>
-      <c r="ACY60" s="35"/>
-      <c r="ACZ60" s="35"/>
-      <c r="ADA60" s="35"/>
-      <c r="ADB60" s="35"/>
-      <c r="ADC60" s="35"/>
-      <c r="ADD60" s="35"/>
-      <c r="ADE60" s="35"/>
-      <c r="ADF60" s="35"/>
-      <c r="ADG60" s="35"/>
-      <c r="ADH60" s="35"/>
-      <c r="ADI60" s="35"/>
-      <c r="ADJ60" s="35"/>
-      <c r="ADK60" s="35"/>
-      <c r="ADL60" s="35"/>
-      <c r="ADM60" s="35"/>
-      <c r="ADN60" s="35"/>
-      <c r="ADO60" s="35"/>
-      <c r="ADP60" s="35"/>
-      <c r="ADQ60" s="35"/>
-      <c r="ADR60" s="35"/>
-      <c r="ADS60" s="35"/>
-      <c r="ADT60" s="35"/>
-      <c r="ADU60" s="35"/>
-      <c r="ADV60" s="35"/>
-      <c r="ADW60" s="35"/>
-      <c r="ADX60" s="35"/>
-      <c r="ADY60" s="35"/>
-      <c r="ADZ60" s="35"/>
-      <c r="AEA60" s="35"/>
-      <c r="AEB60" s="35"/>
-      <c r="AEC60" s="35"/>
-      <c r="AED60" s="35"/>
-      <c r="AEE60" s="35"/>
-      <c r="AEF60" s="35"/>
-      <c r="AEG60" s="35"/>
-      <c r="AEH60" s="35"/>
-      <c r="AEI60" s="35"/>
-      <c r="AEJ60" s="35"/>
-      <c r="AEK60" s="35"/>
-      <c r="AEL60" s="35"/>
-      <c r="AEM60" s="35"/>
-      <c r="AEN60" s="35"/>
-      <c r="AEO60" s="35"/>
-      <c r="AEP60" s="35"/>
-      <c r="AEQ60" s="35"/>
-      <c r="AER60" s="35"/>
-      <c r="AES60" s="35"/>
-      <c r="AET60" s="35"/>
-      <c r="AEU60" s="35"/>
-      <c r="AEV60" s="35"/>
-      <c r="AEW60" s="35"/>
-      <c r="AEX60" s="35"/>
-      <c r="AEY60" s="35"/>
-      <c r="AEZ60" s="35"/>
-      <c r="AFA60" s="35"/>
-      <c r="AFB60" s="35"/>
-      <c r="AFC60" s="35"/>
-      <c r="AFD60" s="35"/>
-      <c r="AFE60" s="35"/>
-      <c r="AFF60" s="35"/>
-      <c r="AFG60" s="35"/>
-      <c r="AFH60" s="35"/>
-      <c r="AFI60" s="35"/>
-      <c r="AFJ60" s="35"/>
-      <c r="AFK60" s="35"/>
-      <c r="AFL60" s="35"/>
-      <c r="AFM60" s="35"/>
-      <c r="AFN60" s="35"/>
-      <c r="AFO60" s="35"/>
-      <c r="AFP60" s="35"/>
-      <c r="AFQ60" s="35"/>
-      <c r="AFR60" s="35"/>
-      <c r="AFS60" s="35"/>
-      <c r="AFT60" s="35"/>
-      <c r="AFU60" s="35"/>
-      <c r="AFV60" s="35"/>
-      <c r="AFW60" s="35"/>
-      <c r="AFX60" s="35"/>
-      <c r="AFY60" s="35"/>
-      <c r="AFZ60" s="35"/>
-      <c r="AGA60" s="35"/>
-      <c r="AGB60" s="35"/>
-      <c r="AGC60" s="35"/>
-      <c r="AGD60" s="35"/>
-      <c r="AGE60" s="35"/>
-      <c r="AGF60" s="35"/>
-      <c r="AGG60" s="35"/>
-      <c r="AGH60" s="35"/>
-      <c r="AGI60" s="35"/>
-      <c r="AGJ60" s="35"/>
-      <c r="AGK60" s="35"/>
-      <c r="AGL60" s="35"/>
-      <c r="AGM60" s="35"/>
-      <c r="AGN60" s="35"/>
-      <c r="AGO60" s="35"/>
-      <c r="AGP60" s="35"/>
-      <c r="AGQ60" s="35"/>
-      <c r="AGR60" s="35"/>
-      <c r="AGS60" s="35"/>
-      <c r="AGT60" s="35"/>
-      <c r="AGU60" s="35"/>
-      <c r="AGV60" s="35"/>
-      <c r="AGW60" s="35"/>
-      <c r="AGX60" s="35"/>
-      <c r="AGY60" s="35"/>
-      <c r="AGZ60" s="35"/>
-      <c r="AHA60" s="35"/>
-      <c r="AHB60" s="35"/>
-      <c r="AHC60" s="35"/>
-      <c r="AHD60" s="35"/>
-      <c r="AHE60" s="35"/>
-      <c r="AHF60" s="35"/>
-      <c r="AHG60" s="35"/>
-      <c r="AHH60" s="35"/>
-      <c r="AHI60" s="35"/>
-      <c r="AHJ60" s="35"/>
-      <c r="AHK60" s="35"/>
-      <c r="AHL60" s="35"/>
-      <c r="AHM60" s="35"/>
-      <c r="AHN60" s="35"/>
-      <c r="AHO60" s="35"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="34"/>
+      <c r="L60" s="34"/>
+      <c r="M60" s="34"/>
+      <c r="N60" s="34"/>
+      <c r="O60" s="34"/>
+      <c r="P60" s="34"/>
+      <c r="Q60" s="34"/>
+      <c r="R60" s="34"/>
+      <c r="S60" s="34"/>
+      <c r="T60" s="34"/>
+      <c r="U60" s="34"/>
+      <c r="V60" s="34"/>
+      <c r="W60" s="34"/>
+      <c r="X60" s="34"/>
+      <c r="Y60" s="34"/>
+      <c r="Z60" s="34"/>
+      <c r="AA60" s="34"/>
+      <c r="AB60" s="34"/>
+      <c r="AC60" s="34"/>
+      <c r="AD60" s="34"/>
+      <c r="AE60" s="34"/>
+      <c r="AF60" s="34"/>
+      <c r="AG60" s="34"/>
+      <c r="AH60" s="34"/>
+      <c r="AI60" s="34"/>
+      <c r="AJ60" s="34"/>
+      <c r="AK60" s="34"/>
+      <c r="AL60" s="34"/>
+      <c r="AM60" s="34"/>
+      <c r="AN60" s="34"/>
+      <c r="AO60" s="34"/>
+      <c r="AP60" s="34"/>
+      <c r="AQ60" s="34"/>
+      <c r="AR60" s="34"/>
+      <c r="AS60" s="34"/>
+      <c r="AT60" s="34"/>
+      <c r="AU60" s="34"/>
+      <c r="AV60" s="34"/>
+      <c r="AW60" s="34"/>
+      <c r="AX60" s="34"/>
+      <c r="AY60" s="34"/>
+      <c r="AZ60" s="34"/>
+      <c r="BA60" s="34"/>
+      <c r="BB60" s="34"/>
+      <c r="BC60" s="34"/>
+      <c r="BD60" s="34"/>
+      <c r="BE60" s="34"/>
+      <c r="BF60" s="34"/>
+      <c r="BG60" s="34"/>
+      <c r="BH60" s="34"/>
+      <c r="BI60" s="34"/>
+      <c r="BJ60" s="34"/>
+      <c r="BK60" s="34"/>
+      <c r="BL60" s="34"/>
+      <c r="BM60" s="34"/>
+      <c r="BN60" s="34"/>
+      <c r="BO60" s="34"/>
+      <c r="BP60" s="34"/>
+      <c r="BQ60" s="34"/>
+      <c r="BR60" s="34"/>
+      <c r="BS60" s="34"/>
+      <c r="BT60" s="34"/>
+      <c r="BU60" s="34"/>
+      <c r="BV60" s="34"/>
+      <c r="BW60" s="34"/>
+      <c r="BX60" s="34"/>
+      <c r="BY60" s="34"/>
+      <c r="BZ60" s="34"/>
+      <c r="CA60" s="34"/>
+      <c r="CB60" s="34"/>
+      <c r="CC60" s="34"/>
+      <c r="CD60" s="34"/>
+      <c r="CE60" s="34"/>
+      <c r="CF60" s="34"/>
+      <c r="CG60" s="34"/>
+      <c r="CH60" s="34"/>
+      <c r="CI60" s="34"/>
+      <c r="CJ60" s="34"/>
+      <c r="CK60" s="34"/>
+      <c r="CL60" s="34"/>
+      <c r="CM60" s="34"/>
+      <c r="CN60" s="34"/>
+      <c r="CO60" s="34"/>
+      <c r="CP60" s="34"/>
+      <c r="CQ60" s="34"/>
+      <c r="CR60" s="34"/>
+      <c r="CS60" s="34"/>
+      <c r="CT60" s="34"/>
+      <c r="CU60" s="34"/>
+      <c r="CV60" s="34"/>
+      <c r="CW60" s="34"/>
+      <c r="CX60" s="34"/>
+      <c r="CY60" s="34"/>
+      <c r="CZ60" s="34"/>
+      <c r="DA60" s="34"/>
+      <c r="DB60" s="34"/>
+      <c r="DC60" s="34"/>
+      <c r="DD60" s="34"/>
+      <c r="DE60" s="34"/>
+      <c r="DF60" s="34"/>
+      <c r="DG60" s="34"/>
+      <c r="DH60" s="34"/>
+      <c r="DI60" s="34"/>
+      <c r="DJ60" s="34"/>
+      <c r="DK60" s="34"/>
+      <c r="DL60" s="34"/>
+      <c r="DM60" s="34"/>
+      <c r="DN60" s="34"/>
+      <c r="DO60" s="34"/>
+      <c r="DP60" s="34"/>
+      <c r="DQ60" s="34"/>
+      <c r="DR60" s="34"/>
+      <c r="DS60" s="34"/>
+      <c r="DT60" s="34"/>
+      <c r="DU60" s="34"/>
+      <c r="DV60" s="34"/>
+      <c r="DW60" s="34"/>
+      <c r="DX60" s="34"/>
+      <c r="DY60" s="34"/>
+      <c r="DZ60" s="34"/>
+      <c r="EA60" s="34"/>
+      <c r="EB60" s="34"/>
+      <c r="EC60" s="34"/>
+      <c r="ED60" s="34"/>
+      <c r="EE60" s="34"/>
+      <c r="EF60" s="34"/>
+      <c r="EG60" s="34"/>
+      <c r="EH60" s="34"/>
+      <c r="EI60" s="34"/>
+      <c r="EJ60" s="34"/>
+      <c r="EK60" s="34"/>
+      <c r="EL60" s="34"/>
+      <c r="EM60" s="34"/>
+      <c r="EN60" s="34"/>
+      <c r="EO60" s="34"/>
+      <c r="EP60" s="34"/>
+      <c r="EQ60" s="34"/>
+      <c r="ER60" s="34"/>
+      <c r="ES60" s="34"/>
+      <c r="ET60" s="34"/>
+      <c r="EU60" s="34"/>
+      <c r="EV60" s="34"/>
+      <c r="EW60" s="34"/>
+      <c r="EX60" s="34"/>
+      <c r="EY60" s="34"/>
+      <c r="EZ60" s="34"/>
+      <c r="FA60" s="34"/>
+      <c r="FB60" s="34"/>
+      <c r="FC60" s="34"/>
+      <c r="FD60" s="34"/>
+      <c r="FE60" s="34"/>
+      <c r="FF60" s="34"/>
+      <c r="FG60" s="34"/>
+      <c r="FH60" s="34"/>
+      <c r="FI60" s="34"/>
+      <c r="FJ60" s="34"/>
+      <c r="FK60" s="34"/>
+      <c r="FL60" s="34"/>
+      <c r="FM60" s="34"/>
+      <c r="FN60" s="34"/>
+      <c r="FO60" s="34"/>
+      <c r="FP60" s="34"/>
+      <c r="FQ60" s="34"/>
+      <c r="FR60" s="34"/>
+      <c r="FS60" s="34"/>
+      <c r="FT60" s="34"/>
+      <c r="FU60" s="34"/>
+      <c r="FV60" s="34"/>
+      <c r="FW60" s="34"/>
+      <c r="FX60" s="34"/>
+      <c r="FY60" s="34"/>
+      <c r="FZ60" s="34"/>
+      <c r="GA60" s="34"/>
+      <c r="GB60" s="34"/>
+      <c r="GC60" s="34"/>
+      <c r="GD60" s="34"/>
+      <c r="GE60" s="34"/>
+      <c r="GF60" s="34"/>
+      <c r="GG60" s="34"/>
+      <c r="GH60" s="34"/>
+      <c r="GI60" s="34"/>
+      <c r="GJ60" s="34"/>
+      <c r="GK60" s="34"/>
+      <c r="GL60" s="34"/>
+      <c r="GM60" s="34"/>
+      <c r="GN60" s="34"/>
+      <c r="GO60" s="34"/>
+      <c r="GP60" s="34"/>
+      <c r="GQ60" s="34"/>
+      <c r="GR60" s="34"/>
+      <c r="GS60" s="34"/>
+      <c r="GT60" s="34"/>
+      <c r="GU60" s="34"/>
+      <c r="GV60" s="34"/>
+      <c r="GW60" s="34"/>
+      <c r="GX60" s="34"/>
+      <c r="GY60" s="34"/>
+      <c r="GZ60" s="34"/>
+      <c r="HA60" s="34"/>
+      <c r="HB60" s="34"/>
+      <c r="HC60" s="34"/>
+      <c r="HD60" s="34"/>
+      <c r="HE60" s="34"/>
+      <c r="HF60" s="34"/>
+      <c r="HG60" s="34"/>
+      <c r="HH60" s="34"/>
+      <c r="HI60" s="34"/>
+      <c r="HJ60" s="34"/>
+      <c r="HK60" s="34"/>
+      <c r="HL60" s="34"/>
+      <c r="HM60" s="34"/>
+      <c r="HN60" s="34"/>
+      <c r="HO60" s="34"/>
+      <c r="HP60" s="34"/>
+      <c r="HQ60" s="34"/>
+      <c r="HR60" s="34"/>
+      <c r="HS60" s="34"/>
+      <c r="HT60" s="34"/>
+      <c r="HU60" s="34"/>
+      <c r="HV60" s="34"/>
+      <c r="HW60" s="34"/>
+      <c r="HX60" s="34"/>
+      <c r="HY60" s="34"/>
+      <c r="HZ60" s="34"/>
+      <c r="IA60" s="34"/>
+      <c r="IB60" s="34"/>
+      <c r="IC60" s="34"/>
+      <c r="ID60" s="34"/>
+      <c r="IE60" s="34"/>
+      <c r="IF60" s="34"/>
+      <c r="IG60" s="34"/>
+      <c r="IH60" s="34"/>
+      <c r="II60" s="34"/>
+      <c r="IJ60" s="34"/>
+      <c r="IK60" s="34"/>
+      <c r="IL60" s="34"/>
+      <c r="IM60" s="34"/>
+      <c r="IN60" s="34"/>
+      <c r="IO60" s="34"/>
+      <c r="IP60" s="34"/>
+      <c r="IQ60" s="34"/>
+      <c r="IR60" s="34"/>
+      <c r="IS60" s="34"/>
+      <c r="IT60" s="34"/>
+      <c r="IU60" s="34"/>
+      <c r="IV60" s="34"/>
+      <c r="IW60" s="34"/>
+      <c r="IX60" s="34"/>
+      <c r="IY60" s="34"/>
+      <c r="IZ60" s="34"/>
+      <c r="JA60" s="34"/>
+      <c r="JB60" s="34"/>
+      <c r="JC60" s="34"/>
+      <c r="JD60" s="34"/>
+      <c r="JE60" s="34"/>
+      <c r="JF60" s="34"/>
+      <c r="JG60" s="34"/>
+      <c r="JH60" s="34"/>
+      <c r="JI60" s="34"/>
+      <c r="JJ60" s="34"/>
+      <c r="JK60" s="34"/>
+      <c r="JL60" s="34"/>
+      <c r="JM60" s="34"/>
+      <c r="JN60" s="34"/>
+      <c r="JO60" s="34"/>
+      <c r="JP60" s="34"/>
+      <c r="JQ60" s="34"/>
+      <c r="JR60" s="34"/>
+      <c r="JS60" s="34"/>
+      <c r="JT60" s="34"/>
+      <c r="JU60" s="34"/>
+      <c r="JV60" s="34"/>
+      <c r="JW60" s="34"/>
+      <c r="JX60" s="34"/>
+      <c r="JY60" s="34"/>
+      <c r="JZ60" s="34"/>
+      <c r="KA60" s="34"/>
+      <c r="KB60" s="34"/>
+      <c r="KC60" s="34"/>
+      <c r="KD60" s="34"/>
+      <c r="KE60" s="34"/>
+      <c r="KF60" s="34"/>
+      <c r="KG60" s="34"/>
+      <c r="KH60" s="34"/>
+      <c r="KI60" s="34"/>
+      <c r="KJ60" s="34"/>
+      <c r="KK60" s="34"/>
+      <c r="KL60" s="34"/>
+      <c r="KM60" s="34"/>
+      <c r="KN60" s="34"/>
+      <c r="KO60" s="34"/>
+      <c r="KP60" s="34"/>
+      <c r="KQ60" s="34"/>
+      <c r="KR60" s="34"/>
+      <c r="KS60" s="34"/>
+      <c r="KT60" s="34"/>
+      <c r="KU60" s="34"/>
+      <c r="KV60" s="34"/>
+      <c r="KW60" s="34"/>
+      <c r="KX60" s="34"/>
+      <c r="KY60" s="34"/>
+      <c r="KZ60" s="34"/>
+      <c r="LA60" s="34"/>
+      <c r="LB60" s="34"/>
+      <c r="LC60" s="34"/>
+      <c r="LD60" s="34"/>
+      <c r="LE60" s="34"/>
+      <c r="LF60" s="34"/>
+      <c r="LG60" s="34"/>
+      <c r="LH60" s="34"/>
+      <c r="LI60" s="34"/>
+      <c r="LJ60" s="34"/>
+      <c r="LK60" s="34"/>
+      <c r="LL60" s="34"/>
+      <c r="LM60" s="34"/>
+      <c r="LN60" s="34"/>
+      <c r="LO60" s="34"/>
+      <c r="LP60" s="34"/>
+      <c r="LQ60" s="34"/>
+      <c r="LR60" s="34"/>
+      <c r="LS60" s="34"/>
+      <c r="LT60" s="34"/>
+      <c r="LU60" s="34"/>
+      <c r="LV60" s="34"/>
+      <c r="LW60" s="34"/>
+      <c r="LX60" s="34"/>
+      <c r="LY60" s="34"/>
+      <c r="LZ60" s="34"/>
+      <c r="MA60" s="34"/>
+      <c r="MB60" s="34"/>
+      <c r="MC60" s="34"/>
+      <c r="MD60" s="34"/>
+      <c r="ME60" s="34"/>
+      <c r="MF60" s="34"/>
+      <c r="MG60" s="34"/>
+      <c r="MH60" s="34"/>
+      <c r="MI60" s="34"/>
+      <c r="MJ60" s="34"/>
+      <c r="MK60" s="34"/>
+      <c r="ML60" s="34"/>
+      <c r="MM60" s="34"/>
+      <c r="MN60" s="34"/>
+      <c r="MO60" s="34"/>
+      <c r="MP60" s="34"/>
+      <c r="MQ60" s="34"/>
+      <c r="MR60" s="34"/>
+      <c r="MS60" s="34"/>
+      <c r="MT60" s="34"/>
+      <c r="MU60" s="34"/>
+      <c r="MV60" s="34"/>
+      <c r="MW60" s="34"/>
+      <c r="MX60" s="34"/>
+      <c r="MY60" s="34"/>
+      <c r="MZ60" s="34"/>
+      <c r="NA60" s="34"/>
+      <c r="NB60" s="34"/>
+      <c r="NC60" s="34"/>
+      <c r="ND60" s="34"/>
+      <c r="NE60" s="34"/>
+      <c r="NF60" s="34"/>
+      <c r="NG60" s="34"/>
+      <c r="NH60" s="34"/>
+      <c r="NI60" s="34"/>
+      <c r="NJ60" s="34"/>
+      <c r="NK60" s="34"/>
+      <c r="NL60" s="34"/>
+      <c r="NM60" s="34"/>
+      <c r="NN60" s="34"/>
+      <c r="NO60" s="34"/>
+      <c r="NP60" s="34"/>
+      <c r="NQ60" s="34"/>
+      <c r="NR60" s="34"/>
+      <c r="NS60" s="34"/>
+      <c r="NT60" s="34"/>
+      <c r="NU60" s="34"/>
+      <c r="NV60" s="34"/>
+      <c r="NW60" s="34"/>
+      <c r="NX60" s="34"/>
+      <c r="NY60" s="34"/>
+      <c r="NZ60" s="34"/>
+      <c r="OA60" s="34"/>
+      <c r="OB60" s="34"/>
+      <c r="OC60" s="34"/>
+      <c r="OD60" s="34"/>
+      <c r="OE60" s="34"/>
+      <c r="OF60" s="34"/>
+      <c r="OG60" s="34"/>
+      <c r="OH60" s="34"/>
+      <c r="OI60" s="34"/>
+      <c r="OJ60" s="34"/>
+      <c r="OK60" s="34"/>
+      <c r="OL60" s="34"/>
+      <c r="OM60" s="34"/>
+      <c r="ON60" s="34"/>
+      <c r="OO60" s="34"/>
+      <c r="OP60" s="34"/>
+      <c r="OQ60" s="34"/>
+      <c r="OR60" s="34"/>
+      <c r="OS60" s="34"/>
+      <c r="OT60" s="34"/>
+      <c r="OU60" s="34"/>
+      <c r="OV60" s="34"/>
+      <c r="OW60" s="34"/>
+      <c r="OX60" s="34"/>
+      <c r="OY60" s="34"/>
+      <c r="OZ60" s="34"/>
+      <c r="PA60" s="34"/>
+      <c r="PB60" s="34"/>
+      <c r="PC60" s="34"/>
+      <c r="PD60" s="34"/>
+      <c r="PE60" s="34"/>
+      <c r="PF60" s="34"/>
+      <c r="PG60" s="34"/>
+      <c r="PH60" s="34"/>
+      <c r="PI60" s="34"/>
+      <c r="PJ60" s="34"/>
+      <c r="PK60" s="34"/>
+      <c r="PL60" s="34"/>
+      <c r="PM60" s="34"/>
+      <c r="PN60" s="34"/>
+      <c r="PO60" s="34"/>
+      <c r="PP60" s="34"/>
+      <c r="PQ60" s="34"/>
+      <c r="PR60" s="34"/>
+      <c r="PS60" s="34"/>
+      <c r="PT60" s="34"/>
+      <c r="PU60" s="34"/>
+      <c r="PV60" s="34"/>
+      <c r="PW60" s="34"/>
+      <c r="PX60" s="34"/>
+      <c r="PY60" s="34"/>
+      <c r="PZ60" s="34"/>
+      <c r="QA60" s="34"/>
+      <c r="QB60" s="34"/>
+      <c r="QC60" s="34"/>
+      <c r="QD60" s="34"/>
+      <c r="QE60" s="34"/>
+      <c r="QF60" s="34"/>
+      <c r="QG60" s="34"/>
+      <c r="QH60" s="34"/>
+      <c r="QI60" s="34"/>
+      <c r="QJ60" s="34"/>
+      <c r="QK60" s="34"/>
+      <c r="QL60" s="34"/>
+      <c r="QM60" s="34"/>
+      <c r="QN60" s="34"/>
+      <c r="QO60" s="34"/>
+      <c r="QP60" s="34"/>
+      <c r="QQ60" s="34"/>
+      <c r="QR60" s="34"/>
+      <c r="QS60" s="34"/>
+      <c r="QT60" s="34"/>
+      <c r="QU60" s="34"/>
+      <c r="QV60" s="34"/>
+      <c r="QW60" s="34"/>
+      <c r="QX60" s="34"/>
+      <c r="QY60" s="34"/>
+      <c r="QZ60" s="34"/>
+      <c r="RA60" s="34"/>
+      <c r="RB60" s="34"/>
+      <c r="RC60" s="34"/>
+      <c r="RD60" s="34"/>
+      <c r="RE60" s="34"/>
+      <c r="RF60" s="34"/>
+      <c r="RG60" s="34"/>
+      <c r="RH60" s="34"/>
+      <c r="RI60" s="34"/>
+      <c r="RJ60" s="34"/>
+      <c r="RK60" s="34"/>
+      <c r="RL60" s="34"/>
+      <c r="RM60" s="34"/>
+      <c r="RN60" s="34"/>
+      <c r="RO60" s="34"/>
+      <c r="RP60" s="34"/>
+      <c r="RQ60" s="34"/>
+      <c r="RR60" s="34"/>
+      <c r="RS60" s="34"/>
+      <c r="RT60" s="34"/>
+      <c r="RU60" s="34"/>
+      <c r="RV60" s="34"/>
+      <c r="RW60" s="34"/>
+      <c r="RX60" s="34"/>
+      <c r="RY60" s="34"/>
+      <c r="RZ60" s="34"/>
+      <c r="SA60" s="34"/>
+      <c r="SB60" s="34"/>
+      <c r="SC60" s="34"/>
+      <c r="SD60" s="34"/>
+      <c r="SE60" s="34"/>
+      <c r="SF60" s="34"/>
+      <c r="SG60" s="34"/>
+      <c r="SH60" s="34"/>
+      <c r="SI60" s="34"/>
+      <c r="SJ60" s="34"/>
+      <c r="SK60" s="34"/>
+      <c r="SL60" s="34"/>
+      <c r="SM60" s="34"/>
+      <c r="SN60" s="34"/>
+      <c r="SO60" s="34"/>
+      <c r="SP60" s="34"/>
+      <c r="SQ60" s="34"/>
+      <c r="SR60" s="34"/>
+      <c r="SS60" s="34"/>
+      <c r="ST60" s="34"/>
+      <c r="SU60" s="34"/>
+      <c r="SV60" s="34"/>
+      <c r="SW60" s="34"/>
+      <c r="SX60" s="34"/>
+      <c r="SY60" s="34"/>
+      <c r="SZ60" s="34"/>
+      <c r="TA60" s="34"/>
+      <c r="TB60" s="34"/>
+      <c r="TC60" s="34"/>
+      <c r="TD60" s="34"/>
+      <c r="TE60" s="34"/>
+      <c r="TF60" s="34"/>
+      <c r="TG60" s="34"/>
+      <c r="TH60" s="34"/>
+      <c r="TI60" s="34"/>
+      <c r="TJ60" s="34"/>
+      <c r="TK60" s="34"/>
+      <c r="TL60" s="34"/>
+      <c r="TM60" s="34"/>
+      <c r="TN60" s="34"/>
+      <c r="TO60" s="34"/>
+      <c r="TP60" s="34"/>
+      <c r="TQ60" s="34"/>
+      <c r="TR60" s="34"/>
+      <c r="TS60" s="34"/>
+      <c r="TT60" s="34"/>
+      <c r="TU60" s="34"/>
+      <c r="TV60" s="34"/>
+      <c r="TW60" s="34"/>
+      <c r="TX60" s="34"/>
+      <c r="TY60" s="34"/>
+      <c r="TZ60" s="34"/>
+      <c r="UA60" s="34"/>
+      <c r="UB60" s="34"/>
+      <c r="UC60" s="34"/>
+      <c r="UD60" s="34"/>
+      <c r="UE60" s="34"/>
+      <c r="UF60" s="34"/>
+      <c r="UG60" s="34"/>
+      <c r="UH60" s="34"/>
+      <c r="UI60" s="34"/>
+      <c r="UJ60" s="34"/>
+      <c r="UK60" s="34"/>
+      <c r="UL60" s="34"/>
+      <c r="UM60" s="34"/>
+      <c r="UN60" s="34"/>
+      <c r="UO60" s="34"/>
+      <c r="UP60" s="34"/>
+      <c r="UQ60" s="34"/>
+      <c r="UR60" s="34"/>
+      <c r="US60" s="34"/>
+      <c r="UT60" s="34"/>
+      <c r="UU60" s="34"/>
+      <c r="UV60" s="34"/>
+      <c r="UW60" s="34"/>
+      <c r="UX60" s="34"/>
+      <c r="UY60" s="34"/>
+      <c r="UZ60" s="34"/>
+      <c r="VA60" s="34"/>
+      <c r="VB60" s="34"/>
+      <c r="VC60" s="34"/>
+      <c r="VD60" s="34"/>
+      <c r="VE60" s="34"/>
+      <c r="VF60" s="34"/>
+      <c r="VG60" s="34"/>
+      <c r="VH60" s="34"/>
+      <c r="VI60" s="34"/>
+      <c r="VJ60" s="34"/>
+      <c r="VK60" s="34"/>
+      <c r="VL60" s="34"/>
+      <c r="VM60" s="34"/>
+      <c r="VN60" s="34"/>
+      <c r="VO60" s="34"/>
+      <c r="VP60" s="34"/>
+      <c r="VQ60" s="34"/>
+      <c r="VR60" s="34"/>
+      <c r="VS60" s="34"/>
+      <c r="VT60" s="34"/>
+      <c r="VU60" s="34"/>
+      <c r="VV60" s="34"/>
+      <c r="VW60" s="34"/>
+      <c r="VX60" s="34"/>
+      <c r="VY60" s="34"/>
+      <c r="VZ60" s="34"/>
+      <c r="WA60" s="34"/>
+      <c r="WB60" s="34"/>
+      <c r="WC60" s="34"/>
+      <c r="WD60" s="34"/>
+      <c r="WE60" s="34"/>
+      <c r="WF60" s="34"/>
+      <c r="WG60" s="34"/>
+      <c r="WH60" s="34"/>
+      <c r="WI60" s="34"/>
+      <c r="WJ60" s="34"/>
+      <c r="WK60" s="34"/>
+      <c r="WL60" s="34"/>
+      <c r="WM60" s="34"/>
+      <c r="WN60" s="34"/>
+      <c r="WO60" s="34"/>
+      <c r="WP60" s="34"/>
+      <c r="WQ60" s="34"/>
+      <c r="WR60" s="34"/>
+      <c r="WS60" s="34"/>
+      <c r="WT60" s="34"/>
+      <c r="WU60" s="34"/>
+      <c r="WV60" s="34"/>
+      <c r="WW60" s="34"/>
+      <c r="WX60" s="34"/>
+      <c r="WY60" s="34"/>
+      <c r="WZ60" s="34"/>
+      <c r="XA60" s="34"/>
+      <c r="XB60" s="34"/>
+      <c r="XC60" s="34"/>
+      <c r="XD60" s="34"/>
+      <c r="XE60" s="34"/>
+      <c r="XF60" s="34"/>
+      <c r="XG60" s="34"/>
+      <c r="XH60" s="34"/>
+      <c r="XI60" s="34"/>
+      <c r="XJ60" s="34"/>
+      <c r="XK60" s="34"/>
+      <c r="XL60" s="34"/>
+      <c r="XM60" s="34"/>
+      <c r="XN60" s="34"/>
+      <c r="XO60" s="34"/>
+      <c r="XP60" s="34"/>
+      <c r="XQ60" s="34"/>
+      <c r="XR60" s="34"/>
+      <c r="XS60" s="34"/>
+      <c r="XT60" s="34"/>
+      <c r="XU60" s="34"/>
+      <c r="XV60" s="34"/>
+      <c r="XW60" s="34"/>
+      <c r="XX60" s="34"/>
+      <c r="XY60" s="34"/>
+      <c r="XZ60" s="34"/>
+      <c r="YA60" s="34"/>
+      <c r="YB60" s="34"/>
+      <c r="YC60" s="34"/>
+      <c r="YD60" s="34"/>
+      <c r="YE60" s="34"/>
+      <c r="YF60" s="34"/>
+      <c r="YG60" s="34"/>
+      <c r="YH60" s="34"/>
+      <c r="YI60" s="34"/>
+      <c r="YJ60" s="34"/>
+      <c r="YK60" s="34"/>
+      <c r="YL60" s="34"/>
+      <c r="YM60" s="34"/>
+      <c r="YN60" s="34"/>
+      <c r="YO60" s="34"/>
+      <c r="YP60" s="34"/>
+      <c r="YQ60" s="34"/>
+      <c r="YR60" s="34"/>
+      <c r="YS60" s="34"/>
+      <c r="YT60" s="34"/>
+      <c r="YU60" s="34"/>
+      <c r="YV60" s="34"/>
+      <c r="YW60" s="34"/>
+      <c r="YX60" s="34"/>
+      <c r="YY60" s="34"/>
+      <c r="YZ60" s="34"/>
+      <c r="ZA60" s="34"/>
+      <c r="ZB60" s="34"/>
+      <c r="ZC60" s="34"/>
+      <c r="ZD60" s="34"/>
+      <c r="ZE60" s="34"/>
+      <c r="ZF60" s="34"/>
+      <c r="ZG60" s="34"/>
+      <c r="ZH60" s="34"/>
+      <c r="ZI60" s="34"/>
+      <c r="ZJ60" s="34"/>
+      <c r="ZK60" s="34"/>
+      <c r="ZL60" s="34"/>
+      <c r="ZM60" s="34"/>
+      <c r="ZN60" s="34"/>
+      <c r="ZO60" s="34"/>
+      <c r="ZP60" s="34"/>
+      <c r="ZQ60" s="34"/>
+      <c r="ZR60" s="34"/>
+      <c r="ZS60" s="34"/>
+      <c r="ZT60" s="34"/>
+      <c r="ZU60" s="34"/>
+      <c r="ZV60" s="34"/>
+      <c r="ZW60" s="34"/>
+      <c r="ZX60" s="34"/>
+      <c r="ZY60" s="34"/>
+      <c r="ZZ60" s="34"/>
+      <c r="AAA60" s="34"/>
+      <c r="AAB60" s="34"/>
+      <c r="AAC60" s="34"/>
+      <c r="AAD60" s="34"/>
+      <c r="AAE60" s="34"/>
+      <c r="AAF60" s="34"/>
+      <c r="AAG60" s="34"/>
+      <c r="AAH60" s="34"/>
+      <c r="AAI60" s="34"/>
+      <c r="AAJ60" s="34"/>
+      <c r="AAK60" s="34"/>
+      <c r="AAL60" s="34"/>
+      <c r="AAM60" s="34"/>
+      <c r="AAN60" s="34"/>
+      <c r="AAO60" s="34"/>
+      <c r="AAP60" s="34"/>
+      <c r="AAQ60" s="34"/>
+      <c r="AAR60" s="34"/>
+      <c r="AAS60" s="34"/>
+      <c r="AAT60" s="34"/>
+      <c r="AAU60" s="34"/>
+      <c r="AAV60" s="34"/>
+      <c r="AAW60" s="34"/>
+      <c r="AAX60" s="34"/>
+      <c r="AAY60" s="34"/>
+      <c r="AAZ60" s="34"/>
+      <c r="ABA60" s="34"/>
+      <c r="ABB60" s="34"/>
+      <c r="ABC60" s="34"/>
+      <c r="ABD60" s="34"/>
+      <c r="ABE60" s="34"/>
+      <c r="ABF60" s="34"/>
+      <c r="ABG60" s="34"/>
+      <c r="ABH60" s="34"/>
+      <c r="ABI60" s="34"/>
+      <c r="ABJ60" s="34"/>
+      <c r="ABK60" s="34"/>
+      <c r="ABL60" s="34"/>
+      <c r="ABM60" s="34"/>
+      <c r="ABN60" s="34"/>
+      <c r="ABO60" s="34"/>
+      <c r="ABP60" s="34"/>
+      <c r="ABQ60" s="34"/>
+      <c r="ABR60" s="34"/>
+      <c r="ABS60" s="34"/>
+      <c r="ABT60" s="34"/>
+      <c r="ABU60" s="34"/>
+      <c r="ABV60" s="34"/>
+      <c r="ABW60" s="34"/>
+      <c r="ABX60" s="34"/>
+      <c r="ABY60" s="34"/>
+      <c r="ABZ60" s="34"/>
+      <c r="ACA60" s="34"/>
+      <c r="ACB60" s="34"/>
+      <c r="ACC60" s="34"/>
+      <c r="ACD60" s="34"/>
+      <c r="ACE60" s="34"/>
+      <c r="ACF60" s="34"/>
+      <c r="ACG60" s="34"/>
+      <c r="ACH60" s="34"/>
+      <c r="ACI60" s="34"/>
+      <c r="ACJ60" s="34"/>
+      <c r="ACK60" s="34"/>
+      <c r="ACL60" s="34"/>
+      <c r="ACM60" s="34"/>
+      <c r="ACN60" s="34"/>
+      <c r="ACO60" s="34"/>
+      <c r="ACP60" s="34"/>
+      <c r="ACQ60" s="34"/>
+      <c r="ACR60" s="34"/>
+      <c r="ACS60" s="34"/>
+      <c r="ACT60" s="34"/>
+      <c r="ACU60" s="34"/>
+      <c r="ACV60" s="34"/>
+      <c r="ACW60" s="34"/>
+      <c r="ACX60" s="34"/>
+      <c r="ACY60" s="34"/>
+      <c r="ACZ60" s="34"/>
+      <c r="ADA60" s="34"/>
+      <c r="ADB60" s="34"/>
+      <c r="ADC60" s="34"/>
+      <c r="ADD60" s="34"/>
+      <c r="ADE60" s="34"/>
+      <c r="ADF60" s="34"/>
+      <c r="ADG60" s="34"/>
+      <c r="ADH60" s="34"/>
+      <c r="ADI60" s="34"/>
+      <c r="ADJ60" s="34"/>
+      <c r="ADK60" s="34"/>
+      <c r="ADL60" s="34"/>
+      <c r="ADM60" s="34"/>
+      <c r="ADN60" s="34"/>
+      <c r="ADO60" s="34"/>
+      <c r="ADP60" s="34"/>
+      <c r="ADQ60" s="34"/>
+      <c r="ADR60" s="34"/>
+      <c r="ADS60" s="34"/>
+      <c r="ADT60" s="34"/>
+      <c r="ADU60" s="34"/>
+      <c r="ADV60" s="34"/>
+      <c r="ADW60" s="34"/>
+      <c r="ADX60" s="34"/>
+      <c r="ADY60" s="34"/>
+      <c r="ADZ60" s="34"/>
+      <c r="AEA60" s="34"/>
+      <c r="AEB60" s="34"/>
+      <c r="AEC60" s="34"/>
+      <c r="AED60" s="34"/>
+      <c r="AEE60" s="34"/>
+      <c r="AEF60" s="34"/>
+      <c r="AEG60" s="34"/>
+      <c r="AEH60" s="34"/>
+      <c r="AEI60" s="34"/>
+      <c r="AEJ60" s="34"/>
+      <c r="AEK60" s="34"/>
+      <c r="AEL60" s="34"/>
+      <c r="AEM60" s="34"/>
+      <c r="AEN60" s="34"/>
+      <c r="AEO60" s="34"/>
+      <c r="AEP60" s="34"/>
+      <c r="AEQ60" s="34"/>
+      <c r="AER60" s="34"/>
+      <c r="AES60" s="34"/>
+      <c r="AET60" s="34"/>
+      <c r="AEU60" s="34"/>
+      <c r="AEV60" s="34"/>
+      <c r="AEW60" s="34"/>
+      <c r="AEX60" s="34"/>
+      <c r="AEY60" s="34"/>
+      <c r="AEZ60" s="34"/>
+      <c r="AFA60" s="34"/>
+      <c r="AFB60" s="34"/>
+      <c r="AFC60" s="34"/>
+      <c r="AFD60" s="34"/>
+      <c r="AFE60" s="34"/>
+      <c r="AFF60" s="34"/>
+      <c r="AFG60" s="34"/>
+      <c r="AFH60" s="34"/>
+      <c r="AFI60" s="34"/>
+      <c r="AFJ60" s="34"/>
+      <c r="AFK60" s="34"/>
+      <c r="AFL60" s="34"/>
+      <c r="AFM60" s="34"/>
+      <c r="AFN60" s="34"/>
+      <c r="AFO60" s="34"/>
+      <c r="AFP60" s="34"/>
+      <c r="AFQ60" s="34"/>
+      <c r="AFR60" s="34"/>
+      <c r="AFS60" s="34"/>
+      <c r="AFT60" s="34"/>
+      <c r="AFU60" s="34"/>
+      <c r="AFV60" s="34"/>
+      <c r="AFW60" s="34"/>
+      <c r="AFX60" s="34"/>
+      <c r="AFY60" s="34"/>
+      <c r="AFZ60" s="34"/>
+      <c r="AGA60" s="34"/>
+      <c r="AGB60" s="34"/>
+      <c r="AGC60" s="34"/>
+      <c r="AGD60" s="34"/>
+      <c r="AGE60" s="34"/>
+      <c r="AGF60" s="34"/>
+      <c r="AGG60" s="34"/>
+      <c r="AGH60" s="34"/>
+      <c r="AGI60" s="34"/>
+      <c r="AGJ60" s="34"/>
+      <c r="AGK60" s="34"/>
+      <c r="AGL60" s="34"/>
+      <c r="AGM60" s="34"/>
+      <c r="AGN60" s="34"/>
+      <c r="AGO60" s="34"/>
+      <c r="AGP60" s="34"/>
+      <c r="AGQ60" s="34"/>
+      <c r="AGR60" s="34"/>
+      <c r="AGS60" s="34"/>
+      <c r="AGT60" s="34"/>
+      <c r="AGU60" s="34"/>
+      <c r="AGV60" s="34"/>
+      <c r="AGW60" s="34"/>
+      <c r="AGX60" s="34"/>
+      <c r="AGY60" s="34"/>
+      <c r="AGZ60" s="34"/>
+      <c r="AHA60" s="34"/>
+      <c r="AHB60" s="34"/>
+      <c r="AHC60" s="34"/>
+      <c r="AHD60" s="34"/>
+      <c r="AHE60" s="34"/>
+      <c r="AHF60" s="34"/>
+      <c r="AHG60" s="34"/>
+      <c r="AHH60" s="34"/>
+      <c r="AHI60" s="34"/>
+      <c r="AHJ60" s="34"/>
+      <c r="AHK60" s="34"/>
+      <c r="AHL60" s="34"/>
+      <c r="AHM60" s="34"/>
+      <c r="AHN60" s="34"/>
+      <c r="AHO60" s="34"/>
       <c r="AHP60" s="33" t="s">
         <v>27</v>
       </c>
@@ -69435,140 +69467,148 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:11842" s="2" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11842" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B61" s="55"/>
-      <c r="C61" s="41" t="s">
+      <c r="B61" s="54"/>
+      <c r="C61" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="D61" s="46" t="s">
+      <c r="D61" s="45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:11842" s="2" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11842" s="2" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="19"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="50"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="49"/>
       <c r="E62" s="21"/>
     </row>
-    <row r="63" spans="1:11842" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11842" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="20"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="51"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="50"/>
     </row>
-    <row r="64" spans="1:11842" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11842" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="53" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="52" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="52" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="51" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="B26:B33"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="B45:B48"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B34:B40"/>
@@ -69585,14 +69625,6 @@
     <mergeCell ref="D52:D55"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B49:B55"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="B26:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -69606,6 +69638,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C252504D64A7FF499891231534EE316A" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2262d1ba7f7e9ea5fc4f552c06531a96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b567ff6e-9321-453e-beed-356cafe9ee74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a68ace85ed6a4dc5d31f3f4a0e20b80" ns3:_="">
     <xsd:import namespace="b567ff6e-9321-453e-beed-356cafe9ee74"/>
@@ -69737,25 +69778,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C61E9DE-9D03-4037-8BF4-6BF9EAF4E4ED}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b567ff6e-9321-453e-beed-356cafe9ee74"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F6FB69-C648-45C8-B8F3-EEA88330BDD4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47F7F8E0-CE34-4040-BE23-F6FCB3B5DFE4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -69771,12 +69818,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F6FB69-C648-45C8-B8F3-EEA88330BDD4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>